<commit_message>
Timesheet updated -gokul & vishnu
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D855EC2-C736-45C0-A38B-C344FD869D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DAEC479F-3822-4219-9D4D-42040ABF32BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="64">
   <si>
     <t>Column1</t>
   </si>
@@ -210,6 +210,9 @@
     <t xml:space="preserve">30 min : Explored Git Desktop,                                                                                                1 hr 15 min : Dependencies and Constraints for management                                                             1hrs 45 mins  :MANAGEMENT Prototype (Dashboard Categories , Pool Members ' Scheduled Interviews Ignored) Refined navigatability                                                                                                   1 hr : Attended  Design Pattern Session                                                                         </t>
   </si>
   <si>
+    <t xml:space="preserve">30 mins : Explored Git                                                    2 hr:  Refined Management Prototype                         1hr : Attended Design Pattern Session(Builder and Protoype)                                                                              1hr : Softskills                                                                  </t>
+  </si>
+  <si>
     <t>Dependencies for Interviewer (7-13)</t>
   </si>
   <si>
@@ -219,7 +222,7 @@
     <t xml:space="preserve">2 hr : Correction in Interviewer Prototype                                                                                                                             1 hr : Redefined Prototype for interviewer and management                                                                                               1.5 hr : Attended Design patternSession                                                                                                            1 hr : Aligned Interviewer and management      Prototype                                                                      </t>
   </si>
   <si>
-    <t xml:space="preserve">Exploring on </t>
+    <t>Exploring on Git and Git Desktop</t>
   </si>
   <si>
     <t xml:space="preserve">2 hr: Creating prototype for admin using FIGMA                                                                            1.5 hr : Attending Design pattern session (Prototype and Builder design)                                                                  1 hr : preparing for review and self exploration                                           2 hr: Understanding the overall flow, Ensuring changes which were said yesterday(Drop down for project,Phone number and role, scroll page,back button,adding filter,interview denied list.) </t>
@@ -3274,8 +3277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF90A9D-38BA-40BE-8A97-FB9144A9E457}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3441,7 +3444,7 @@
       </c>
       <c r="H10" s="24"/>
     </row>
-    <row r="11" spans="1:8" ht="409.6">
+    <row r="11" spans="1:8" ht="214.5" customHeight="1">
       <c r="B11" s="19" t="s">
         <v>21</v>
       </c>
@@ -3449,16 +3452,16 @@
         <v>39</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="E11" s="35" t="s">
         <v>16</v>
       </c>
       <c r="F11" s="35">
-        <v>6</v>
+        <v>2.5</v>
       </c>
       <c r="G11" s="35">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H11" s="25"/>
     </row>
@@ -3488,10 +3491,10 @@
         <v>27</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D13" s="44" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>41</v>
@@ -3546,7 +3549,7 @@
         <v>52</v>
       </c>
       <c r="D16" s="43" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E16" s="35" t="s">
         <v>41</v>
@@ -3564,10 +3567,10 @@
         <v>54</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E17" s="42" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Time Sheet Updated - Deepika
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DAEC479F-3822-4219-9D4D-42040ABF32BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D518F2A-1F2A-4EA9-AD85-0A108DCA5A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="66">
   <si>
     <t>Column1</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t xml:space="preserve">30 min : Explored Git Desktop,                                                                                                1 hr 15 min : Dependencies and Constraints for management                                                             1hrs 45 mins  :MANAGEMENT Prototype (Dashboard Categories , Pool Members ' Scheduled Interviews Ignored) Refined navigatability                                                                                                   1 hr : Attended  Design Pattern Session                                                                         </t>
+  </si>
+  <si>
+    <t>Prototype for current flow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 hr           : Constraints for TAC                                                                                             1hr            :  Attended Design Pattern Session                                                                                                                  1 hr           :  Prototype for Current drive ,Upcoming drive                                                                                 1 hr           :  Prototype for Create Invite                                                                                                                                      </t>
   </si>
   <si>
     <t xml:space="preserve">30 mins : Explored Git                                                    2 hr:  Refined Management Prototype                         1hr : Attended Design Pattern Session(Builder and Protoype)                                                                              1hr : Softskills                                                                  </t>
@@ -3277,8 +3283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF90A9D-38BA-40BE-8A97-FB9144A9E457}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3423,21 +3429,21 @@
       </c>
       <c r="H9" s="24"/>
     </row>
-    <row r="10" spans="1:8" ht="409.6">
+    <row r="10" spans="1:8" ht="103.5">
       <c r="B10" s="19" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="E10" s="35" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="35">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="G10" s="35">
         <v>1</v>
@@ -3452,7 +3458,7 @@
         <v>39</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E11" s="35" t="s">
         <v>16</v>
@@ -3491,10 +3497,10 @@
         <v>27</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D13" s="44" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>41</v>
@@ -3549,7 +3555,7 @@
         <v>52</v>
       </c>
       <c r="D16" s="43" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E16" s="35" t="s">
         <v>41</v>
@@ -3567,10 +3573,10 @@
         <v>54</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E17" s="42" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Timesheet updated - darshana,sheik and remuki
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25203"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D518F2A-1F2A-4EA9-AD85-0A108DCA5A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A9C3A54-DF15-4D31-ABF8-AB764D4898F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="72">
   <si>
     <t>Column1</t>
   </si>
@@ -210,6 +210,12 @@
     <t xml:space="preserve">30 min : Explored Git Desktop,                                                                                                1 hr 15 min : Dependencies and Constraints for management                                                             1hrs 45 mins  :MANAGEMENT Prototype (Dashboard Categories , Pool Members ' Scheduled Interviews Ignored) Refined navigatability                                                                                                   1 hr : Attended  Design Pattern Session                                                                         </t>
   </si>
   <si>
+    <t xml:space="preserve">Prototype </t>
+  </si>
+  <si>
+    <t>Acceptance criteria for TAC-1hr                                       Design pattern session -1hr                                               Refinded TAC prototype- 2hr                                         Design pattern -30 min</t>
+  </si>
+  <si>
     <t>Prototype for current flow</t>
   </si>
   <si>
@@ -223,6 +229,18 @@
   </si>
   <si>
     <t>1hr :  Explored git and git desktop                          1hr :  Refined Prototype for Interviewer-Dashboard                                                              1hr : Attended Design pattern Session(Builder and Prototype pattern)                                                                         1hr : Refined Prototype for Interviewer                          1hr : Acceptence criteria and constrains for interviewer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 hr  :  Dependencies for TAC                                       1 hr  :  Prototype for TAC ,Create pool ,Manage pool                                                                                      1 hr  :  Attended Design Pattern Session                    1 hr   : Soft Skills Session                                                1 hr  : Prototype for TAC                                                                                                                                                                                                                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                                                                                                                                </t>
+  </si>
+  <si>
+    <t>Acceptence(8-13) , Dependencies(8-13) for interviewers, Prototype</t>
+  </si>
+  <si>
+    <t>30 mins :  Explored git and git desktop                          1hr :  Refined Prototype for Interviewer-10 slide  1hr : Attended Design pattern Session(Builder and Prototype pattern)                                                                         1hr : Refined Prototype for Interviewer                             1 hr : soft skill sessions</t>
   </si>
   <si>
     <t xml:space="preserve">2 hr : Correction in Interviewer Prototype                                                                                                                             1 hr : Redefined Prototype for interviewer and management                                                                                               1.5 hr : Attended Design patternSession                                                                                                            1 hr : Aligned Interviewer and management      Prototype                                                                      </t>
@@ -3283,8 +3301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF90A9D-38BA-40BE-8A97-FB9144A9E457}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3408,19 +3426,17 @@
       </c>
       <c r="H8" s="23"/>
     </row>
-    <row r="9" spans="1:8" ht="409.6">
+    <row r="9" spans="1:8" ht="83.25">
       <c r="B9" s="19" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="35" t="s">
-        <v>16</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="E9" s="35"/>
       <c r="F9" s="35">
         <v>4.5</v>
       </c>
@@ -3434,14 +3450,12 @@
         <v>20</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="35" t="s">
-        <v>16</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="E10" s="35"/>
       <c r="F10" s="35">
         <v>4</v>
       </c>
@@ -3458,7 +3472,7 @@
         <v>39</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E11" s="35" t="s">
         <v>16</v>
@@ -3497,10 +3511,10 @@
         <v>27</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D13" s="44" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>41</v>
@@ -3513,34 +3527,38 @@
       </c>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:8" ht="165.75">
+    <row r="14" spans="1:8" ht="103.5">
       <c r="B14" s="19" t="s">
         <v>30</v>
       </c>
       <c r="C14" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="35"/>
+      <c r="D14" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>66</v>
+      </c>
       <c r="F14" s="35"/>
       <c r="G14" s="35"/>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:8" ht="409.6">
+    <row r="15" spans="1:8" ht="124.5">
       <c r="B15" s="19" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="E15" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F15" s="35">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="G15" s="35" t="s">
         <v>41</v>
@@ -3555,7 +3573,7 @@
         <v>52</v>
       </c>
       <c r="D16" s="43" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E16" s="35" t="s">
         <v>41</v>
@@ -3573,10 +3591,10 @@
         <v>54</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E17" s="42" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Timesheet updated - Kumaresh
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A9C3A54-DF15-4D31-ABF8-AB764D4898F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0DB9107A-0BE6-490A-9695-9CC36AF764CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="73">
   <si>
     <t>Column1</t>
   </si>
@@ -223,6 +223,13 @@
   </si>
   <si>
     <t xml:space="preserve">30 mins : Explored Git                                                    2 hr:  Refined Management Prototype                         1hr : Attended Design Pattern Session(Builder and Protoype)                                                                              1hr : Softskills                                                                  </t>
+  </si>
+  <si>
+    <t>30 Mins: Explored Github Desktop
+1 Hr 30 Mins: Refined Prototype for Interviewer
+1 Hr: Design pattern session(Builder and Prototype)
+1 Hr: Softskills session 
+1 Hr 30 Mins: Refined Management Prototype and its flow.</t>
   </si>
   <si>
     <t>Dependencies for Interviewer (7-13)</t>
@@ -3301,8 +3308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF90A9D-38BA-40BE-8A97-FB9144A9E457}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3485,24 +3492,24 @@
       </c>
       <c r="H11" s="25"/>
     </row>
-    <row r="12" spans="1:8" ht="189">
+    <row r="12" spans="1:8" ht="189.75" customHeight="1">
       <c r="B12" s="19" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="E12" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F12" s="35">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="G12" s="35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12" s="25"/>
     </row>
@@ -3511,10 +3518,10 @@
         <v>27</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D13" s="44" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>41</v>
@@ -3535,10 +3542,10 @@
         <v>49</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="35"/>
@@ -3549,10 +3556,10 @@
         <v>31</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E15" s="35" t="s">
         <v>41</v>
@@ -3573,7 +3580,7 @@
         <v>52</v>
       </c>
       <c r="D16" s="43" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E16" s="35" t="s">
         <v>41</v>
@@ -3591,10 +3598,10 @@
         <v>54</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E17" s="42" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
UPDATED TIME SHEET - SHEIK FAREETH H
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{697140EF-DD98-4017-9EF0-B493036DAE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{62CC8A1C-0865-4060-AC56-E42AFD5BCE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="83">
   <si>
     <t>Column1</t>
   </si>
@@ -284,6 +284,11 @@
   </si>
   <si>
     <t xml:space="preserve"> 30 min :BrainStroming                                                      1 hr : Dependencies for TAC                                          1 hr :  Prototype for TAC</t>
+  </si>
+  <si>
+    <t>30 mins : Brain stroming
+1 hr : Refining the Interviewers Prototype ( Dash board , Profile , Navigations )
+1 hr : TAC ( Creating pools , Pool details prototype , and refining Slide )</t>
   </si>
   <si>
     <t xml:space="preserve">Exploring on Data models </t>
@@ -560,7 +565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -685,6 +690,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4221,8 +4229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF90A9D-38BA-40BE-8A97-FB9144A9E457}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4445,7 +4453,7 @@
       </c>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:8" ht="62.25">
+    <row r="14" spans="1:8" ht="84">
       <c r="B14" s="19" t="s">
         <v>30</v>
       </c>
@@ -4466,7 +4474,7 @@
       </c>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:8" ht="124.5">
+    <row r="15" spans="1:8" ht="105">
       <c r="B15" s="19" t="s">
         <v>31</v>
       </c>
@@ -4474,13 +4482,13 @@
         <v>68</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E15" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="35">
-        <v>4.5</v>
+      <c r="F15" s="45">
+        <v>2.5</v>
       </c>
       <c r="G15" s="35" t="s">
         <v>41</v>
@@ -4513,10 +4521,10 @@
         <v>54</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E17" s="42" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Updated Timesheet - Prithviraj
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25203"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62CC8A1C-0865-4060-AC56-E42AFD5BCE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6129321E-7D1E-4C32-9F2A-05FD97DBB6E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="86">
   <si>
     <t>Column1</t>
   </si>
@@ -260,6 +260,9 @@
     <t xml:space="preserve">2 hr: Creating prototype for admin using FIGMA                                                                            1.5 hr : Attending Design pattern session (Prototype and Builder design)                                                                  1 hr : preparing for review and self exploration                                           2 hr: Understanding the overall flow, Ensuring changes which were said yesterday(Drop down for project,Phone number and role, scroll page,back button,adding filter,interview denied list.) </t>
   </si>
   <si>
+    <t>Absent</t>
+  </si>
+  <si>
     <t>Data  Model</t>
   </si>
   <si>
@@ -281,6 +284,14 @@
   <si>
     <t>30 min: Brain Storming with team                                  1.5 hr: Refined management Prototype
 30 min: Refined management and interviewer prototype(alignment)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dependencies for Interviewer (7-13),Data Modelling </t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 mins : Brain stroming with Team
+1 hr : Refining the TAC Prototype ( Dash board , Profile )
+30 mins : TAC Prototype Page Alignments               30 mins : Refined TAC Prototype (Home page)  </t>
   </si>
   <si>
     <t xml:space="preserve"> 30 min :BrainStroming                                                      1 hr : Dependencies for TAC                                          1 hr :  Prototype for TAC</t>
@@ -4229,8 +4240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF90A9D-38BA-40BE-8A97-FB9144A9E457}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4333,38 +4344,40 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="144.75">
+    <row r="8" spans="1:8" ht="21">
       <c r="B8" s="19" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="E8" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F8" s="35">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G8" s="35">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="H8" s="23"/>
     </row>
-    <row r="9" spans="1:8" ht="62.25">
+    <row r="9" spans="1:8" ht="84">
       <c r="B9" s="19" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="E9" s="35"/>
+        <v>75</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>41</v>
+      </c>
       <c r="F9" s="35">
         <v>1</v>
       </c>
@@ -4373,17 +4386,19 @@
       </c>
       <c r="H9" s="24"/>
     </row>
-    <row r="10" spans="1:8" ht="83.25">
+    <row r="10" spans="1:8" ht="105">
       <c r="B10" s="19" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="E10" s="35"/>
+        <v>77</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>41</v>
+      </c>
       <c r="F10" s="35">
         <v>2.5</v>
       </c>
@@ -4397,12 +4412,14 @@
         <v>21</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="E11" s="35"/>
+        <v>78</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>41</v>
+      </c>
       <c r="F11" s="35">
         <v>2.5</v>
       </c>
@@ -4416,10 +4433,10 @@
         <v>24</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E12" s="35" t="s">
         <v>41</v>
@@ -4437,23 +4454,23 @@
         <v>27</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="D13" s="44" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F13" s="35">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="G13" s="35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:8" ht="84">
+    <row r="14" spans="1:8" ht="63">
       <c r="B14" s="19" t="s">
         <v>30</v>
       </c>
@@ -4461,16 +4478,16 @@
         <v>49</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>67</v>
+        <v>82</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>41</v>
       </c>
       <c r="F14" s="35">
         <v>2.5</v>
       </c>
-      <c r="G14" s="35" t="s">
-        <v>41</v>
+      <c r="G14" s="35">
+        <v>0</v>
       </c>
       <c r="H14" s="25"/>
     </row>
@@ -4482,7 +4499,7 @@
         <v>68</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E15" s="35" t="s">
         <v>41</v>
@@ -4490,12 +4507,12 @@
       <c r="F15" s="45">
         <v>2.5</v>
       </c>
-      <c r="G15" s="35" t="s">
-        <v>41</v>
+      <c r="G15" s="35">
+        <v>0</v>
       </c>
       <c r="H15" s="26"/>
     </row>
-    <row r="16" spans="1:8" ht="124.5">
+    <row r="16" spans="1:8" ht="189">
       <c r="B16" s="19" t="s">
         <v>34</v>
       </c>
@@ -4521,12 +4538,12 @@
         <v>54</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F17" s="42">

</xml_diff>

<commit_message>
updated timesheet_ vishnu prakaash R
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7FAB6F5-AAB5-421B-8E95-2A58C69B8288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB7CA9F2-31E8-4D6F-8FE8-1255889C7AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="94">
   <si>
     <t>Column1</t>
   </si>
@@ -334,6 +334,12 @@
   </si>
   <si>
     <t>1 Hr 30 Mins: Brainstorming  with team                                           1 Hr 30 mins:Data Modelling(Overview,Response table)                                                                                1 Hr : Refined Data-Model(Added Invites ,Response Type table)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1hr: Brainstorming with Team
+45m: Adding pages and refining flow on ADMIN access.
+45m: Entered attribute values for drive and discussing logic with Team mates.
+30m: College project discussion - review call </t>
   </si>
 </sst>
 </file>
@@ -5154,8 +5160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1698D63-CC5D-425D-9D4F-258DF9281991}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5447,24 +5453,24 @@
       </c>
       <c r="H16" s="27"/>
     </row>
-    <row r="17" spans="2:8" ht="83.25">
+    <row r="17" spans="2:8" ht="126">
       <c r="B17" s="21" t="s">
         <v>54</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="E17" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F17" s="42">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="G17" s="42">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="H17" s="28"/>
     </row>

</xml_diff>

<commit_message>
Update Timesheet - Kumaresh
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24CF7951-2827-408C-8958-26C85F2FF6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F410E59-D159-4FF3-8EB2-792A91212AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="96">
   <si>
     <t>Column1</t>
   </si>
@@ -328,6 +328,9 @@
   </si>
   <si>
     <t>1Hr 30Mins:Brainstorming                                              2Hr:Data Model(7 Entities)</t>
+  </si>
+  <si>
+    <t>1 Hr 30 Mins: Brainstorming  with team                                           1 Hr :Refined User Stories,Acceptance Criteria        1 Hr 30 Mins :Refined Dependancies and Constraints(Management,Interviewer)</t>
   </si>
   <si>
     <t xml:space="preserve">Refine Data Model(Should add Interface) </t>
@@ -5166,8 +5169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1698D63-CC5D-425D-9D4F-258DF9281991}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5362,13 +5365,13 @@
         <v>76</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="E12" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F12" s="35">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="G12" s="35">
         <v>0</v>
@@ -5380,10 +5383,10 @@
         <v>27</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D13" s="44" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>41</v>
@@ -5404,7 +5407,7 @@
         <v>49</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E14" s="35" t="s">
         <v>41</v>
@@ -5467,7 +5470,7 @@
         <v>41</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E17" s="35" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Updated Time sheet - Sheik Fareeth
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F410E59-D159-4FF3-8EB2-792A91212AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A42C8462-5039-4555-A800-4360E1BA84BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="DAY 4(07-04-2022)" sheetId="42" r:id="rId2"/>
     <sheet name="DAY 5 (08-04-2022) (2)" sheetId="44" r:id="rId3"/>
     <sheet name="DAY 6 (09-04-2022)" sheetId="43" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="45" r:id="rId5"/>
+    <sheet name="Day 7 (11-04-2022)" sheetId="45" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="97">
   <si>
     <t>Column1</t>
   </si>
@@ -323,8 +323,8 @@
   </si>
   <si>
     <t>1 Hr 30 mins : Brainstorming with team
-1 Hr 30 mins : Prototype for TAC-(Create,View &amp; Delete Pool)
-1 Hr         : Redefined the overall flow of TAC</t>
+1 Hr 30 mins : Prototype for TAC-(Create,View &amp; Delete Pool -  6 slides)
+1 Hr         : Redefined the overall prototype for TAC</t>
   </si>
   <si>
     <t>1Hr 30Mins:Brainstorming                                              2Hr:Data Model(7 Entities)</t>
@@ -343,6 +343,12 @@
  2 hr    : Refined the Prototype for TAC ( Edit pool )
  30 minutes    : Alligingment.        
 </t>
+  </si>
+  <si>
+    <t>1 hr - Brain Stromming
+30 Mins - Adding New slides to TAC ( Upcoming drives, notifications, scheduling drives - 5 slides )
+2 hr - Building Data model In draw.io ( 7 Entities )
+30 Mins - Re refining Interviewers scheduled drive cancellation</t>
   </si>
   <si>
     <t xml:space="preserve">1hr: Brainstorming with Team
@@ -5169,8 +5175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1698D63-CC5D-425D-9D4F-258DF9281991}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5273,7 +5279,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="83.25">
+    <row r="8" spans="1:8" ht="103.5" customHeight="1">
       <c r="B8" s="19" t="s">
         <v>13</v>
       </c>
@@ -5294,7 +5300,7 @@
       </c>
       <c r="H8" s="23"/>
     </row>
-    <row r="9" spans="1:8" ht="84">
+    <row r="9" spans="1:8" ht="99" customHeight="1">
       <c r="B9" s="19" t="s">
         <v>17</v>
       </c>
@@ -5315,7 +5321,7 @@
       </c>
       <c r="H9" s="24"/>
     </row>
-    <row r="10" spans="1:8" ht="83.25">
+    <row r="10" spans="1:8" ht="102.75" customHeight="1">
       <c r="B10" s="19" t="s">
         <v>20</v>
       </c>
@@ -5336,7 +5342,7 @@
       </c>
       <c r="H10" s="24"/>
     </row>
-    <row r="11" spans="1:8" ht="214.5" customHeight="1">
+    <row r="11" spans="1:8" ht="116.25" customHeight="1">
       <c r="B11" s="19" t="s">
         <v>21</v>
       </c>
@@ -5350,14 +5356,14 @@
         <v>41</v>
       </c>
       <c r="F11" s="35">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="G11" s="35">
         <v>0</v>
       </c>
       <c r="H11" s="25"/>
     </row>
-    <row r="12" spans="1:8" ht="189.75" customHeight="1">
+    <row r="12" spans="1:8" ht="133.5" customHeight="1">
       <c r="B12" s="19" t="s">
         <v>24</v>
       </c>
@@ -5378,7 +5384,7 @@
       </c>
       <c r="H12" s="25"/>
     </row>
-    <row r="13" spans="1:8" ht="205.5" customHeight="1">
+    <row r="13" spans="1:8" ht="133.5" customHeight="1">
       <c r="B13" s="19" t="s">
         <v>27</v>
       </c>
@@ -5404,7 +5410,7 @@
         <v>30</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>94</v>
@@ -5420,28 +5426,28 @@
       </c>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:8" ht="103.5">
+    <row r="15" spans="1:8" ht="144" customHeight="1">
       <c r="B15" s="19" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="E15" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F15" s="45">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="G15" s="35">
         <v>0</v>
       </c>
       <c r="H15" s="26"/>
     </row>
-    <row r="16" spans="1:8" ht="83.25">
+    <row r="16" spans="1:8" ht="111" customHeight="1">
       <c r="B16" s="19" t="s">
         <v>34</v>
       </c>
@@ -5462,21 +5468,21 @@
       </c>
       <c r="H16" s="27"/>
     </row>
-    <row r="17" spans="2:8" ht="126">
+    <row r="17" spans="2:8" ht="142.5" customHeight="1">
       <c r="B17" s="21" t="s">
         <v>54</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E17" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F17" s="42">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="G17" s="42">
         <v>0.5</v>

</xml_diff>

<commit_message>
Updated timesheet - vishnu prakaash R
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0441430F-1250-42BF-897F-87457CFF2D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5C40AEE-C77C-414A-B310-7AAE097F281B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="106">
   <si>
     <t>Column1</t>
   </si>
@@ -387,6 +387,11 @@
     <t xml:space="preserve">1Hr 30 mins : Brainstroming
 1 Hr 30 mins : Corrections done in TAC
 30 mins : Discussed design pattern                                                            </t>
+  </si>
+  <si>
+    <t>1.5 HR: BrainStorming with Team
+1 HR: Refined Admin Flow (Added pool deletion request from TAC)
+1 HR: ANGULAR - self exploration</t>
   </si>
 </sst>
 </file>
@@ -6093,8 +6098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1698D63-CC5D-425D-9D4F-258DF9281991}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6394,16 +6399,16 @@
         <v>76</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="E17" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F17" s="42">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="G17" s="42">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H17" s="28"/>
     </row>

</xml_diff>

<commit_message>
Updated Timesheet-Gokul P ,Sheik Fareeth
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{087DD833-6697-47C6-BAF9-94AE37001B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{303FFF8F-7147-4BF4-90BD-1507BEDF3DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="110">
   <si>
     <t>Column1</t>
   </si>
@@ -376,6 +376,9 @@
 2 Hrs              : Entered Attribute values for Project &amp; Drives </t>
   </si>
   <si>
+    <t>1hr 30mins:Brain stroming with team                                                       1hr30mins: Refined Datamodel(response and cancellation)                                                                       30mins:session with anitha</t>
+  </si>
+  <si>
     <t xml:space="preserve">Refine Data Model(Should add Interface,Relationship) </t>
   </si>
   <si>
@@ -385,6 +388,10 @@
     <t xml:space="preserve"> 1 hr 30 minutes : Brainstroming with the team
 1 hr          :  Preparing for the Review 
 1 hr 30 min   :  Data Entry for Available member Table. </t>
+  </si>
+  <si>
+    <t>1 hr 30 mins - Brain Stromming
+45mins:Preparing for  code review                                     45mins :attending review                                                30mins:session with anitha</t>
   </si>
   <si>
     <t>Data Modeling(Methods)</t>
@@ -6104,8 +6111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1698D63-CC5D-425D-9D4F-258DF9281991}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6279,7 +6286,7 @@
         <v>76</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="E11" s="35" t="s">
         <v>41</v>
@@ -6299,9 +6306,7 @@
       <c r="C12" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="13" t="s">
-        <v>91</v>
-      </c>
+      <c r="D12" s="13"/>
       <c r="E12" s="35" t="s">
         <v>41</v>
       </c>
@@ -6318,10 +6323,10 @@
         <v>27</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D13" s="44" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>41</v>
@@ -6342,7 +6347,7 @@
         <v>76</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E14" s="35" t="s">
         <v>41</v>
@@ -6363,13 +6368,13 @@
         <v>76</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="E15" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F15" s="45">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="G15" s="35">
         <v>0</v>
@@ -6381,10 +6386,10 @@
         <v>34</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D16" s="43" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E16" s="35" t="s">
         <v>41</v>
@@ -6405,7 +6410,7 @@
         <v>76</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E17" s="35" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Updated Timesheet _ Vishnu Prakaash R
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B05706F-B52E-4F01-9D42-97ADD86A07C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B535A9F-2B42-4860-A2D7-44D9F3D310AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="126">
   <si>
     <t>Column1</t>
   </si>
@@ -462,9 +462,20 @@
     <t xml:space="preserve">1 Hr : Brainstorming with team                                    1 Hr 30 mins: Session with Rafi(Data modeling)          1 Hr : Explored normalization concepts                          1 Hr : Edited data model tables </t>
   </si>
   <si>
-    <t>1.5 HR: BrainStorming with Team
-1 HR: Refined Admin Flow (Added pool deletion request from TAC)
-1 HR: ANGULAR - self exploration</t>
+    <t xml:space="preserve">Angular:Architecture, components and Templates.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1 hr : Brainstorming with Team Mates
+1.5 hr : Angular pakage installation (rxjs,schematics/update) and version update.
+15 mins : Break 
+1 hr : Admin flow - Evaluation and Novelty
+15 mins :  The Hindu article - NEWS
+1.5 hr : General Session (GOALS) - with Rafi
+15 mins :  IDLE
+1 hr : Lunch Break 
+15 mins : Pushed updated timesheet on GIT.</t>
   </si>
 </sst>
 </file>
@@ -7067,8 +7078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1698D63-CC5D-425D-9D4F-258DF9281991}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7339,7 +7350,7 @@
       </c>
       <c r="H15" s="26"/>
     </row>
-    <row r="16" spans="1:8" ht="142.5" customHeight="1">
+    <row r="16" spans="1:8" ht="146.25" customHeight="1">
       <c r="B16" s="19" t="s">
         <v>34</v>
       </c>
@@ -7360,15 +7371,15 @@
       </c>
       <c r="H16" s="27"/>
     </row>
-    <row r="17" spans="2:8" ht="142.5" customHeight="1">
+    <row r="17" spans="2:8" ht="268.5" customHeight="1">
       <c r="B17" s="21" t="s">
         <v>54</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>76</v>
+        <v>124</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E17" s="35" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Updated Timesheet - Kumaresh
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86890B9D-C42E-416B-A6C6-F40DCDD1BF0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDC4A15D-4861-4D6D-84DC-B1852861A854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="128">
   <si>
     <t>Column1</t>
   </si>
@@ -433,8 +433,13 @@
     <t>1hr 30mins:Brain stroming with team                                                       1hr30mins: Refined Datamodel(response and cancellation)                                                                       30mins:session with anitha</t>
   </si>
   <si>
-    <t>1 hr 30 mins - Brain Stromming
-1Hr:Preparing for  code review                                     1hr :Attending review                                                30mins:session with anitha</t>
+    <t>Exploring (HTML,CSS,JAVASCRIPT)</t>
+  </si>
+  <si>
+    <t>1hr : Brainstorming with team
+1hr : Redefined TAC Prototype (Add project,Remove Project,Alligned Navigation bar)
+1hr 30m:Attended Raffi Sessions
+1hr : Datamodel Operations(Employee)</t>
   </si>
   <si>
     <t>1 Hr 30 Mins: Brainstorming  with team                                           1 Hr 30 mins:Refined Data Modelling(Interview,EmployeeResponse table)                                                                                30 Mins : Added Data-Model(Added Cancelled Interview, Cancellation type table)</t>
@@ -7083,8 +7088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1698D63-CC5D-425D-9D4F-258DF9281991}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7276,19 +7281,19 @@
         <v>24</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>76</v>
+        <v>117</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E12" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F12" s="35">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="G12" s="35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="25"/>
     </row>
@@ -7300,7 +7305,7 @@
         <v>104</v>
       </c>
       <c r="D13" s="44" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>41</v>
@@ -7318,10 +7323,10 @@
         <v>30</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E14" s="35" t="s">
         <v>41</v>
@@ -7339,10 +7344,10 @@
         <v>31</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D15" s="47" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E15" s="35" t="s">
         <v>41</v>
@@ -7360,10 +7365,10 @@
         <v>34</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D16" s="44" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E16" s="35" t="s">
         <v>41</v>
@@ -7381,19 +7386,19 @@
         <v>54</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E17" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F17" s="42">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="G17" s="42">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H17" s="28"/>
     </row>

</xml_diff>

<commit_message>
Updated Time sheet - Deepika
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25217"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F7AF013-6D69-4EB1-B268-13497600A8B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B9497E4-F415-4858-9C67-C4CFCB3C60CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="139">
   <si>
     <t>Column1</t>
   </si>
@@ -506,7 +506,16 @@
 15 mins : Pushed updated timesheet on GIT.</t>
   </si>
   <si>
-    <t>1 hr-Brainstorming with team                                              1hr-HTTP protocol                                                                  1hr-Web API                                                                            1hr-Written services for TAC                                                 1 hr-TypeScript</t>
+    <t>1 hr-Brainstorming with team                                              1hr-HTTP protocol                                                                  1hr-Explored Web API                                                                            1hr-Written services for TAC                                                 1 hr-Exploration TypeScript</t>
+  </si>
+  <si>
+    <t>Preparation of High Level Design, Typescript</t>
+  </si>
+  <si>
+    <t>1 Hr: Brainstorming with Team
+1 Hr 30 mins : Exploration on Javascript &amp; Typescript
+1 Hr : Worked on Designing Layout
+1 Hr 30 mins : Written Services for Interviewer &amp; TAC</t>
   </si>
   <si>
     <t>High Level Design</t>
@@ -8024,7 +8033,7 @@
   <dimension ref="A2:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8158,11 +8167,9 @@
         <v>41</v>
       </c>
       <c r="F9" s="35">
-        <v>2.5</v>
-      </c>
-      <c r="G9" s="35">
-        <v>1.5</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G9" s="35"/>
       <c r="H9" s="24"/>
     </row>
     <row r="10" spans="1:8" ht="147" customHeight="1">
@@ -8170,20 +8177,18 @@
         <v>20</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="E10" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F10" s="35">
-        <v>3</v>
-      </c>
-      <c r="G10" s="35">
-        <v>1</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G10" s="35"/>
       <c r="H10" s="24"/>
     </row>
     <row r="11" spans="1:8" ht="229.5" customHeight="1">
@@ -8233,10 +8238,10 @@
         <v>27</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D13" s="44" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>41</v>
@@ -8278,7 +8283,7 @@
         <v>125</v>
       </c>
       <c r="D15" s="47" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E15" s="35" t="s">
         <v>41</v>
@@ -8296,10 +8301,10 @@
         <v>34</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D16" s="44" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E16" s="35" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Updated Timesheet - Vishnu, Remuki
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0AD252B-9440-4DA8-A63E-FBF16BC50853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2D4BD47-7192-4D82-88FD-8C3BB0BFF2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="148">
   <si>
     <t>Column1</t>
   </si>
@@ -552,6 +552,11 @@
 </t>
   </si>
   <si>
+    <t>1 hour               :  Brainstorming
+30 minutes    : Exploring HTML
+30 minutes      : Exploring CSS                                              1 hour           : Exploring on Javascript and TypeScript               1 hour              :Exploring on WEB API</t>
+  </si>
+  <si>
     <t>PROJECT :
 Brain Storming with team - 1 hr                                           Exploring basics of VS Code - 1.5 hr                                        Exploring basics of Asp.net MVC Core - 1 hr
 Exploring basics of Javascript - 30 mins                               Listing out the Services for Users (TAC, Interviewer ) - 1 hr</t>
@@ -565,6 +570,15 @@
 1 hr : exploration on entity framework
 1 hr : Tried migration on code first approach 
 1 hr : exploration on typescript</t>
+  </si>
+  <si>
+    <t>Layout creation and Implementation</t>
+  </si>
+  <si>
+    <t>1 hr - Brainstorming with Team mates
+2 hr - Angular (Data binding and Directives)
+2 hr - Typescript(Basic syntac, variables,Types and Operators)
+0.5 hr - HLD Sample Documentation - overall view</t>
   </si>
 </sst>
 </file>
@@ -8055,8 +8069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F34C89B-AD9F-4621-B8F8-86D1460206B9}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8285,16 +8299,16 @@
         <v>123</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="E14" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F14" s="35">
-        <v>3.5</v>
-      </c>
-      <c r="G14" s="35">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="G14" s="35" t="s">
+        <v>41</v>
       </c>
       <c r="H14" s="25"/>
     </row>
@@ -8306,7 +8320,7 @@
         <v>125</v>
       </c>
       <c r="D15" s="47" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E15" s="35" t="s">
         <v>41</v>
@@ -8324,10 +8338,10 @@
         <v>34</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D16" s="44" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E16" s="35" t="s">
         <v>41</v>
@@ -8345,19 +8359,19 @@
         <v>54</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="E17" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F17" s="42">
-        <v>2</v>
-      </c>
-      <c r="G17" s="42">
-        <v>5</v>
+        <v>5.5</v>
+      </c>
+      <c r="G17" s="42" t="s">
+        <v>41</v>
       </c>
       <c r="H17" s="28"/>
     </row>

</xml_diff>

<commit_message>
Timesheet updated - Vinoth
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2D4BD47-7192-4D82-88FD-8C3BB0BFF2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{68499DDD-4B65-4B7B-93D5-562FAD6A96CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 3(06-04-2022)" sheetId="40" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Day 8 (12-04-2022)" sheetId="48" r:id="rId6"/>
     <sheet name="Day 9 (13-04-2022)" sheetId="45" r:id="rId7"/>
     <sheet name="Day10 ( 18-04-2022 )" sheetId="49" r:id="rId8"/>
+    <sheet name="Day11 ( 19-04-2022 )" sheetId="51" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="151">
   <si>
     <t>Column1</t>
   </si>
@@ -566,7 +567,7 @@
   </si>
   <si>
     <t>1 hr : Brainstorming
-2 hr : exploration on web api core
+2 hr : exploration on webapi
 1 hr : exploration on entity framework
 1 hr : Tried migration on code first approach 
 1 hr : exploration on typescript</t>
@@ -579,6 +580,17 @@
 2 hr - Angular (Data binding and Directives)
 2 hr - Typescript(Basic syntac, variables,Types and Operators)
 0.5 hr - HLD Sample Documentation - overall view</t>
+  </si>
+  <si>
+    <t>Angular</t>
+  </si>
+  <si>
+    <t>1 hr : Brainstorming
+2 hr : exploration on angular basics
+1 hr : exploration on entity framework                              1 hr : exploration on angular components</t>
+  </si>
+  <si>
+    <t>1 hr : Attented Review  with Anitha</t>
   </si>
 </sst>
 </file>
@@ -986,7 +998,539 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="168">
+  <dxfs count="189">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="16"/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="16"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -5257,232 +5801,261 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B59126C7-EF4B-42B8-885B-D999B591F622}" name="Table2" displayName="Table2" ref="B9:H19" totalsRowShown="0" headerRowDxfId="167" dataDxfId="166" headerRowBorderDxfId="164" tableBorderDxfId="165" totalsRowBorderDxfId="163">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B59126C7-EF4B-42B8-885B-D999B591F622}" name="Table2" displayName="Table2" ref="B9:H19" totalsRowShown="0" headerRowDxfId="188" dataDxfId="187" headerRowBorderDxfId="185" tableBorderDxfId="186" totalsRowBorderDxfId="184">
   <autoFilter ref="B9:H19" xr:uid="{B59126C7-EF4B-42B8-885B-D999B591F622}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{52B5F38B-ABB3-47C0-BB3D-A29F2DE51CC7}" name="Resource Name" dataDxfId="162"/>
-    <tableColumn id="2" xr3:uid="{EE1FCD6C-E5A0-4CCC-B385-C1EFECE5FDAA}" name="In-progress" dataDxfId="161"/>
-    <tableColumn id="3" xr3:uid="{181E4433-047B-4DE4-8CA4-63F4C195E21B}" name="Done" dataDxfId="160"/>
-    <tableColumn id="4" xr3:uid="{3D6F0A13-3C98-4A4C-A37F-39C4F130B0FD}" name="Discarded / Hold" dataDxfId="159"/>
-    <tableColumn id="5" xr3:uid="{6C95647F-EC05-4637-9771-13884C172508}" name="Hours Spent - Project" dataDxfId="158"/>
-    <tableColumn id="6" xr3:uid="{61429939-C632-43F5-B197-7173C32B4F6F}" name="Hours Spent - Non Project" dataDxfId="157"/>
-    <tableColumn id="7" xr3:uid="{FA348B8C-B11C-46EA-A9B6-9E454AA967AA}" name="Comments" dataDxfId="156"/>
+    <tableColumn id="1" xr3:uid="{52B5F38B-ABB3-47C0-BB3D-A29F2DE51CC7}" name="Resource Name" dataDxfId="183"/>
+    <tableColumn id="2" xr3:uid="{EE1FCD6C-E5A0-4CCC-B385-C1EFECE5FDAA}" name="In-progress" dataDxfId="182"/>
+    <tableColumn id="3" xr3:uid="{181E4433-047B-4DE4-8CA4-63F4C195E21B}" name="Done" dataDxfId="181"/>
+    <tableColumn id="4" xr3:uid="{3D6F0A13-3C98-4A4C-A37F-39C4F130B0FD}" name="Discarded / Hold" dataDxfId="180"/>
+    <tableColumn id="5" xr3:uid="{6C95647F-EC05-4637-9771-13884C172508}" name="Hours Spent - Project" dataDxfId="179"/>
+    <tableColumn id="6" xr3:uid="{61429939-C632-43F5-B197-7173C32B4F6F}" name="Hours Spent - Non Project" dataDxfId="178"/>
+    <tableColumn id="7" xr3:uid="{FA348B8C-B11C-46EA-A9B6-9E454AA967AA}" name="Comments" dataDxfId="177"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D14697CD-D871-4BE9-9957-83E5498C6EE5}" name="Table3751113" displayName="Table3751113" ref="B2:E4" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70" headerRowBorderDxfId="68" tableBorderDxfId="69" totalsRowBorderDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D14697CD-D871-4BE9-9957-83E5498C6EE5}" name="Table3751113" displayName="Table3751113" ref="B2:E4" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91" headerRowBorderDxfId="89" tableBorderDxfId="90" totalsRowBorderDxfId="88">
   <autoFilter ref="B2:E4" xr:uid="{9D11D6AC-943D-4BD1-9800-DECD246F6E62}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{597AD08F-5CEE-486B-928A-4E0143DEB21C}" name="Column1" dataDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{80BDA1F7-DDA4-494F-BB7E-61D9A6E30A98}" name="Column2" dataDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{DF109DE4-28E3-4BB2-997F-34A3F319520E}" name="Column3" dataDxfId="64"/>
-    <tableColumn id="4" xr3:uid="{C98D2CDB-0DA6-4DBC-80D8-197F6DC8262F}" name="Column4" dataDxfId="63"/>
+    <tableColumn id="1" xr3:uid="{597AD08F-5CEE-486B-928A-4E0143DEB21C}" name="Column1" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{80BDA1F7-DDA4-494F-BB7E-61D9A6E30A98}" name="Column2" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{DF109DE4-28E3-4BB2-997F-34A3F319520E}" name="Column3" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{C98D2CDB-0DA6-4DBC-80D8-197F6DC8262F}" name="Column4" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{A036296C-A09A-4538-8AEF-52AAB9228500}" name="Table2621014" displayName="Table2621014" ref="B7:H17" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61" headerRowBorderDxfId="59" tableBorderDxfId="60" totalsRowBorderDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{A036296C-A09A-4538-8AEF-52AAB9228500}" name="Table2621014" displayName="Table2621014" ref="B7:H17" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82" headerRowBorderDxfId="80" tableBorderDxfId="81" totalsRowBorderDxfId="79">
   <autoFilter ref="B7:H17" xr:uid="{A30D6EFF-9BA6-4C4E-A49E-6E01C92313FC}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{AF106EC2-9249-449D-84E6-7F225A50644A}" name="Resource Name" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{C5721F56-75DD-416B-8AF4-882B78C097A4}" name="In-progress" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{65371F98-F64C-4B19-8CA2-7EF266D44FBF}" name="Done" dataDxfId="55"/>
-    <tableColumn id="4" xr3:uid="{EDCBD646-6D4A-4D8E-A78F-13A92C55A829}" name="Discarded / Hold" dataDxfId="54"/>
-    <tableColumn id="5" xr3:uid="{5216518A-9337-493A-8FBE-8BB58C828250}" name="Hours Spent - Project" dataDxfId="53"/>
-    <tableColumn id="6" xr3:uid="{249FD4AA-FDB0-40B3-A254-56EFA2226474}" name="Hours Spent - Non Project" dataDxfId="52"/>
-    <tableColumn id="7" xr3:uid="{47669AF2-CA1E-4E4D-8758-1BE493ED8AF4}" name="Comments" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{AF106EC2-9249-449D-84E6-7F225A50644A}" name="Resource Name" dataDxfId="78"/>
+    <tableColumn id="2" xr3:uid="{C5721F56-75DD-416B-8AF4-882B78C097A4}" name="In-progress" dataDxfId="77"/>
+    <tableColumn id="3" xr3:uid="{65371F98-F64C-4B19-8CA2-7EF266D44FBF}" name="Done" dataDxfId="76"/>
+    <tableColumn id="4" xr3:uid="{EDCBD646-6D4A-4D8E-A78F-13A92C55A829}" name="Discarded / Hold" dataDxfId="75"/>
+    <tableColumn id="5" xr3:uid="{5216518A-9337-493A-8FBE-8BB58C828250}" name="Hours Spent - Project" dataDxfId="74"/>
+    <tableColumn id="6" xr3:uid="{249FD4AA-FDB0-40B3-A254-56EFA2226474}" name="Hours Spent - Non Project" dataDxfId="73"/>
+    <tableColumn id="7" xr3:uid="{47669AF2-CA1E-4E4D-8758-1BE493ED8AF4}" name="Comments" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{7FA1E999-6830-41E9-8136-B3DD83876559}" name="Table3751115" displayName="Table3751115" ref="B2:E4" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49" headerRowBorderDxfId="47" tableBorderDxfId="48" totalsRowBorderDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{7FA1E999-6830-41E9-8136-B3DD83876559}" name="Table3751115" displayName="Table3751115" ref="B2:E4" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70" headerRowBorderDxfId="68" tableBorderDxfId="69" totalsRowBorderDxfId="67">
   <autoFilter ref="B2:E4" xr:uid="{9D11D6AC-943D-4BD1-9800-DECD246F6E62}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D67A75C6-50A5-4ED9-9562-707A5D717E14}" name="Column1" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{4CBEA24E-4C4B-4B23-85EB-4A8217A30752}" name="Column2" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{A13B37EF-4736-411C-BF75-CBDF316BAB90}" name="Column3" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{504EFC7F-2F49-4D22-ACB4-DCD4F1C95FE1}" name="Column4" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{D67A75C6-50A5-4ED9-9562-707A5D717E14}" name="Column1" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{4CBEA24E-4C4B-4B23-85EB-4A8217A30752}" name="Column2" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{A13B37EF-4736-411C-BF75-CBDF316BAB90}" name="Column3" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{504EFC7F-2F49-4D22-ACB4-DCD4F1C95FE1}" name="Column4" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A30D6EFF-9BA6-4C4E-A49E-6E01C92313FC}" name="Table26210" displayName="Table26210" ref="B7:H17" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" headerRowBorderDxfId="38" tableBorderDxfId="39" totalsRowBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A30D6EFF-9BA6-4C4E-A49E-6E01C92313FC}" name="Table26210" displayName="Table26210" ref="B7:H17" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61" headerRowBorderDxfId="59" tableBorderDxfId="60" totalsRowBorderDxfId="58">
   <autoFilter ref="B7:H17" xr:uid="{A30D6EFF-9BA6-4C4E-A49E-6E01C92313FC}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{CB514E32-07C5-40CB-B6EC-7CE1D7B57BF0}" name="Resource Name" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{C46C6E29-0824-4E17-8EAF-64A911996B4D}" name="In-progress" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{6B5DC81A-7A98-4BF7-864C-E5A79BB97505}" name="Done" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{0C243582-3F95-4A38-8545-76DB2898625E}" name="Discarded / Hold" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{FD3CD380-CAB0-422C-8CF7-6944378DDBE6}" name="Hours Spent - Project" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{145CB7BA-3D9C-44AC-9E51-716B58B77D2F}" name="Hours Spent - Non Project" dataDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{507AE42A-A1CC-4934-90C2-3BFCE53238B3}" name="Comments" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{CB514E32-07C5-40CB-B6EC-7CE1D7B57BF0}" name="Resource Name" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{C46C6E29-0824-4E17-8EAF-64A911996B4D}" name="In-progress" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{6B5DC81A-7A98-4BF7-864C-E5A79BB97505}" name="Done" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{0C243582-3F95-4A38-8545-76DB2898625E}" name="Discarded / Hold" dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{FD3CD380-CAB0-422C-8CF7-6944378DDBE6}" name="Hours Spent - Project" dataDxfId="53"/>
+    <tableColumn id="6" xr3:uid="{145CB7BA-3D9C-44AC-9E51-716B58B77D2F}" name="Hours Spent - Non Project" dataDxfId="52"/>
+    <tableColumn id="7" xr3:uid="{507AE42A-A1CC-4934-90C2-3BFCE53238B3}" name="Comments" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9D11D6AC-943D-4BD1-9800-DECD246F6E62}" name="Table37511" displayName="Table37511" ref="B2:E4" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" headerRowBorderDxfId="26" tableBorderDxfId="27" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9D11D6AC-943D-4BD1-9800-DECD246F6E62}" name="Table37511" displayName="Table37511" ref="B2:E4" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49" headerRowBorderDxfId="47" tableBorderDxfId="48" totalsRowBorderDxfId="46">
   <autoFilter ref="B2:E4" xr:uid="{9D11D6AC-943D-4BD1-9800-DECD246F6E62}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6B075576-4726-42C8-996A-A7B4B187D27F}" name="Column1" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{2B0F43B9-480B-4C54-A4CC-3DFC00711929}" name="Column2" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{4353F121-13EC-4653-AB7A-C0BBED71F612}" name="Column3" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{AD8279C5-6226-4ECF-A6C8-F9C70974EABE}" name="Column4" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{6B075576-4726-42C8-996A-A7B4B187D27F}" name="Column1" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{2B0F43B9-480B-4C54-A4CC-3DFC00711929}" name="Column2" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{4353F121-13EC-4653-AB7A-C0BBED71F612}" name="Column3" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{AD8279C5-6226-4ECF-A6C8-F9C70974EABE}" name="Column4" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{1356D4E1-15F0-41BF-B0C4-E4DC18B96A83}" name="Table2621016" displayName="Table2621016" ref="B7:H17" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{1356D4E1-15F0-41BF-B0C4-E4DC18B96A83}" name="Table2621016" displayName="Table2621016" ref="B7:H17" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" headerRowBorderDxfId="38" tableBorderDxfId="39" totalsRowBorderDxfId="37">
   <autoFilter ref="B7:H17" xr:uid="{1356D4E1-15F0-41BF-B0C4-E4DC18B96A83}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{975CF6D7-F24C-4D9F-BA9F-439AF60EF114}" name="Resource Name" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{BC36331B-5C09-49F2-8E13-D5168DD28D0F}" name="In-progress" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{41B5A763-B80D-4E4B-976F-9969D2C0C14F}" name="Done" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{5D1F40BB-F239-4A1D-AEF6-82A5FC99D7CD}" name="Discarded / Hold" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{5C9549F2-9CF2-45B7-98E8-1D291B3630B2}" name="Hours Spent - Project" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{04DC6A6C-EEB6-4EF4-911D-C37E2C5B40FF}" name="Hours Spent - Non Project" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{C3902E87-CCB6-47C9-9BC1-FD0B37543238}" name="Comments" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{975CF6D7-F24C-4D9F-BA9F-439AF60EF114}" name="Resource Name" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{BC36331B-5C09-49F2-8E13-D5168DD28D0F}" name="In-progress" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{41B5A763-B80D-4E4B-976F-9969D2C0C14F}" name="Done" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{5D1F40BB-F239-4A1D-AEF6-82A5FC99D7CD}" name="Discarded / Hold" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{5C9549F2-9CF2-45B7-98E8-1D291B3630B2}" name="Hours Spent - Project" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{04DC6A6C-EEB6-4EF4-911D-C37E2C5B40FF}" name="Hours Spent - Non Project" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{C3902E87-CCB6-47C9-9BC1-FD0B37543238}" name="Comments" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E3497E54-1E59-44E7-9480-106E98FB838A}" name="Table3751117" displayName="Table3751117" ref="B2:E4" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E3497E54-1E59-44E7-9480-106E98FB838A}" name="Table3751117" displayName="Table3751117" ref="B2:E4" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" headerRowBorderDxfId="26" tableBorderDxfId="27" totalsRowBorderDxfId="25">
   <autoFilter ref="B2:E4" xr:uid="{E3497E54-1E59-44E7-9480-106E98FB838A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{69E7B7B7-0FF3-43D1-AE4A-578CB3CCCFBD}" name="Column1" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{753FC1E8-1B96-4804-A794-92A8953D5EE2}" name="Column2" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{50B38A4B-BAF8-4640-8ECB-0900A6C915DB}" name="Column3" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{4432DCD0-98FF-4B59-BAB7-E3FE0A3EDFBC}" name="Column4" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{69E7B7B7-0FF3-43D1-AE4A-578CB3CCCFBD}" name="Column1" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{753FC1E8-1B96-4804-A794-92A8953D5EE2}" name="Column2" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{50B38A4B-BAF8-4640-8ECB-0900A6C915DB}" name="Column3" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{4432DCD0-98FF-4B59-BAB7-E3FE0A3EDFBC}" name="Column4" dataDxfId="21"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{D3490739-1854-4802-BC7E-8F8A56938939}" name="Table262101618" displayName="Table262101618" ref="B7:H17" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+  <autoFilter ref="B7:H17" xr:uid="{1356D4E1-15F0-41BF-B0C4-E4DC18B96A83}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{F4CDC508-938F-4C7B-9D78-6C7897C95C75}" name="Resource Name" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{D24B5720-9179-4EA6-A1B2-11FFE3971AE0}" name="In-progress" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{38376D7D-1777-43ED-87F4-271C7CA93BC0}" name="Done" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{27CF804E-18A7-4ED9-9891-7FE4B93C6D6C}" name="Discarded / Hold" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{F23FF8B6-B301-4C5F-ACF3-3D16EEFFC3F0}" name="Hours Spent - Project" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{2D0142DB-38B6-4D6B-A60F-A9A19574C7ED}" name="Hours Spent - Non Project" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{8BAC7AAB-A572-4256-AFEE-71DC94CC59B9}" name="Comments" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{65B9F601-45A2-418D-921A-3D56A32B6C21}" name="Table375111719" displayName="Table375111719" ref="B2:E4" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+  <autoFilter ref="B2:E4" xr:uid="{E3497E54-1E59-44E7-9480-106E98FB838A}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{6E252E52-03A5-4570-990A-B3378296E039}" name="Column1" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{D5447885-EF1E-44FE-B1A4-EE1475056221}" name="Column2" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{2F816DC6-3307-4F6E-9962-EB8AB2F91C9F}" name="Column3" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{21AE6030-4E77-45A3-8CDA-342E87194417}" name="Column4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BF3C43CE-B630-4202-BD3A-6EE2D770899A}" name="Table3" displayName="Table3" ref="B4:E6" totalsRowShown="0" headerRowDxfId="155" dataDxfId="154" headerRowBorderDxfId="152" tableBorderDxfId="153" totalsRowBorderDxfId="151">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BF3C43CE-B630-4202-BD3A-6EE2D770899A}" name="Table3" displayName="Table3" ref="B4:E6" totalsRowShown="0" headerRowDxfId="176" dataDxfId="175" headerRowBorderDxfId="173" tableBorderDxfId="174" totalsRowBorderDxfId="172">
   <autoFilter ref="B4:E6" xr:uid="{BF3C43CE-B630-4202-BD3A-6EE2D770899A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BE43EB49-4D5D-488E-9520-6CE4AC2E5C1B}" name="Column1" dataDxfId="150"/>
-    <tableColumn id="2" xr3:uid="{16DFD0E6-4C5E-443C-BF24-706A867EF798}" name="Column2" dataDxfId="149"/>
-    <tableColumn id="3" xr3:uid="{DC8A145E-C833-4BE6-BAE5-7E5E2AC2891C}" name="Column3" dataDxfId="148"/>
-    <tableColumn id="4" xr3:uid="{9454D612-74D7-428F-B9A0-7151862F7C2A}" name="Column4" dataDxfId="147"/>
+    <tableColumn id="1" xr3:uid="{BE43EB49-4D5D-488E-9520-6CE4AC2E5C1B}" name="Column1" dataDxfId="171"/>
+    <tableColumn id="2" xr3:uid="{16DFD0E6-4C5E-443C-BF24-706A867EF798}" name="Column2" dataDxfId="170"/>
+    <tableColumn id="3" xr3:uid="{DC8A145E-C833-4BE6-BAE5-7E5E2AC2891C}" name="Column3" dataDxfId="169"/>
+    <tableColumn id="4" xr3:uid="{9454D612-74D7-428F-B9A0-7151862F7C2A}" name="Column4" dataDxfId="168"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{46BFD46F-1AD6-4EF9-9F4D-9841A6E71CD9}" name="Table26" displayName="Table26" ref="B8:H18" totalsRowShown="0" headerRowDxfId="146" dataDxfId="145" headerRowBorderDxfId="143" tableBorderDxfId="144" totalsRowBorderDxfId="142">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{46BFD46F-1AD6-4EF9-9F4D-9841A6E71CD9}" name="Table26" displayName="Table26" ref="B8:H18" totalsRowShown="0" headerRowDxfId="167" dataDxfId="166" headerRowBorderDxfId="164" tableBorderDxfId="165" totalsRowBorderDxfId="163">
   <autoFilter ref="B8:H18" xr:uid="{46BFD46F-1AD6-4EF9-9F4D-9841A6E71CD9}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{7428D5F6-9EE3-49C6-B1BE-E57BFF59C7B0}" name="Resource Name" dataDxfId="141"/>
-    <tableColumn id="2" xr3:uid="{8EF82413-9CDB-4809-98BD-913D08316031}" name="In-progress" dataDxfId="140"/>
-    <tableColumn id="3" xr3:uid="{B4E2F1CC-113D-4DBD-9D8F-AFFEF819725B}" name="Done" dataDxfId="139"/>
-    <tableColumn id="4" xr3:uid="{A8C1C667-3FF8-4B7C-AEC8-2DD543708DEA}" name="Discarded / Hold" dataDxfId="138"/>
-    <tableColumn id="5" xr3:uid="{DF5599B4-665D-4C1C-8DFF-80F68FB27D64}" name="Hours Spent - Project" dataDxfId="137"/>
-    <tableColumn id="6" xr3:uid="{EAD7742A-CE22-40A8-90BD-AB0C0555FA39}" name="Hours Spent - Non Project" dataDxfId="136"/>
-    <tableColumn id="7" xr3:uid="{52C2DA4C-9FFA-48AF-B36A-2837B9ED00F1}" name="Comments" dataDxfId="135"/>
+    <tableColumn id="1" xr3:uid="{7428D5F6-9EE3-49C6-B1BE-E57BFF59C7B0}" name="Resource Name" dataDxfId="162"/>
+    <tableColumn id="2" xr3:uid="{8EF82413-9CDB-4809-98BD-913D08316031}" name="In-progress" dataDxfId="161"/>
+    <tableColumn id="3" xr3:uid="{B4E2F1CC-113D-4DBD-9D8F-AFFEF819725B}" name="Done" dataDxfId="160"/>
+    <tableColumn id="4" xr3:uid="{A8C1C667-3FF8-4B7C-AEC8-2DD543708DEA}" name="Discarded / Hold" dataDxfId="159"/>
+    <tableColumn id="5" xr3:uid="{DF5599B4-665D-4C1C-8DFF-80F68FB27D64}" name="Hours Spent - Project" dataDxfId="158"/>
+    <tableColumn id="6" xr3:uid="{EAD7742A-CE22-40A8-90BD-AB0C0555FA39}" name="Hours Spent - Non Project" dataDxfId="157"/>
+    <tableColumn id="7" xr3:uid="{52C2DA4C-9FFA-48AF-B36A-2837B9ED00F1}" name="Comments" dataDxfId="156"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9997EBAF-6A71-418E-B851-C8B1915211B5}" name="Table37" displayName="Table37" ref="B3:E5" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133" headerRowBorderDxfId="131" tableBorderDxfId="132" totalsRowBorderDxfId="130">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9997EBAF-6A71-418E-B851-C8B1915211B5}" name="Table37" displayName="Table37" ref="B3:E5" totalsRowShown="0" headerRowDxfId="155" dataDxfId="154" headerRowBorderDxfId="152" tableBorderDxfId="153" totalsRowBorderDxfId="151">
   <autoFilter ref="B3:E5" xr:uid="{9997EBAF-6A71-418E-B851-C8B1915211B5}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{7EDDA488-2881-4A15-9B9C-777D834D815F}" name="Column1" dataDxfId="129"/>
-    <tableColumn id="2" xr3:uid="{AFE02A3A-062D-4251-90A2-DA5D33B35508}" name="Column2" dataDxfId="128"/>
-    <tableColumn id="3" xr3:uid="{ED8EDBC8-15CC-4013-9D78-2DF925F82DCD}" name="Column3" dataDxfId="127"/>
-    <tableColumn id="4" xr3:uid="{62C95B61-46F3-42F7-A1B8-B69D37DD10DF}" name="Column4" dataDxfId="126"/>
+    <tableColumn id="1" xr3:uid="{7EDDA488-2881-4A15-9B9C-777D834D815F}" name="Column1" dataDxfId="150"/>
+    <tableColumn id="2" xr3:uid="{AFE02A3A-062D-4251-90A2-DA5D33B35508}" name="Column2" dataDxfId="149"/>
+    <tableColumn id="3" xr3:uid="{ED8EDBC8-15CC-4013-9D78-2DF925F82DCD}" name="Column3" dataDxfId="148"/>
+    <tableColumn id="4" xr3:uid="{62C95B61-46F3-42F7-A1B8-B69D37DD10DF}" name="Column4" dataDxfId="147"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{158FF28A-C282-456C-9B5E-C00624BAAA83}" name="Table2628" displayName="Table2628" ref="B7:H17" totalsRowShown="0" headerRowDxfId="125" dataDxfId="124" headerRowBorderDxfId="122" tableBorderDxfId="123" totalsRowBorderDxfId="121">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{158FF28A-C282-456C-9B5E-C00624BAAA83}" name="Table2628" displayName="Table2628" ref="B7:H17" totalsRowShown="0" headerRowDxfId="146" dataDxfId="145" headerRowBorderDxfId="143" tableBorderDxfId="144" totalsRowBorderDxfId="142">
   <autoFilter ref="B7:H17" xr:uid="{B1AE0DC9-D1F6-4E81-8D21-EBCF5F00B2B7}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{FA7FB678-9F12-498D-AC8C-EA3804FA6C35}" name="Resource Name" dataDxfId="120"/>
-    <tableColumn id="2" xr3:uid="{393B2B95-8815-4457-B760-B5E70FBBB0A5}" name="In-progress" dataDxfId="119"/>
-    <tableColumn id="3" xr3:uid="{400FD95F-D628-4B07-904B-1F5E11C584A9}" name="Done" dataDxfId="118"/>
-    <tableColumn id="4" xr3:uid="{DA6CAF01-4620-4AD9-8F22-C26934025345}" name="Discarded / Hold" dataDxfId="117"/>
-    <tableColumn id="5" xr3:uid="{D70C3DC4-AF79-4EA9-916E-2DDB8181B077}" name="Hours Spent - Project" dataDxfId="116"/>
-    <tableColumn id="6" xr3:uid="{BA92211F-9DF3-4897-86C0-5FE2D8FC9C28}" name="Hours Spent - Non Project" dataDxfId="115"/>
-    <tableColumn id="7" xr3:uid="{673B654E-8412-4BCE-9293-22370300F740}" name="Comments" dataDxfId="114"/>
+    <tableColumn id="1" xr3:uid="{FA7FB678-9F12-498D-AC8C-EA3804FA6C35}" name="Resource Name" dataDxfId="141"/>
+    <tableColumn id="2" xr3:uid="{393B2B95-8815-4457-B760-B5E70FBBB0A5}" name="In-progress" dataDxfId="140"/>
+    <tableColumn id="3" xr3:uid="{400FD95F-D628-4B07-904B-1F5E11C584A9}" name="Done" dataDxfId="139"/>
+    <tableColumn id="4" xr3:uid="{DA6CAF01-4620-4AD9-8F22-C26934025345}" name="Discarded / Hold" dataDxfId="138"/>
+    <tableColumn id="5" xr3:uid="{D70C3DC4-AF79-4EA9-916E-2DDB8181B077}" name="Hours Spent - Project" dataDxfId="137"/>
+    <tableColumn id="6" xr3:uid="{BA92211F-9DF3-4897-86C0-5FE2D8FC9C28}" name="Hours Spent - Non Project" dataDxfId="136"/>
+    <tableColumn id="7" xr3:uid="{673B654E-8412-4BCE-9293-22370300F740}" name="Comments" dataDxfId="135"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FE979438-BC3B-45D4-9D8F-CD3DAC132734}" name="Table3759" displayName="Table3759" ref="B2:E4" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112" headerRowBorderDxfId="110" tableBorderDxfId="111" totalsRowBorderDxfId="109">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FE979438-BC3B-45D4-9D8F-CD3DAC132734}" name="Table3759" displayName="Table3759" ref="B2:E4" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133" headerRowBorderDxfId="131" tableBorderDxfId="132" totalsRowBorderDxfId="130">
   <autoFilter ref="B2:E4" xr:uid="{ACFFF651-B126-4B94-92B4-F3166A18744A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D1B206E0-BC18-44C3-AC3A-E386EBC240DA}" name="Column1" dataDxfId="108"/>
-    <tableColumn id="2" xr3:uid="{93DD1EAA-9879-4D36-9385-C9A727E59F3F}" name="Column2" dataDxfId="107"/>
-    <tableColumn id="3" xr3:uid="{C1074E65-5D51-4E3A-B9B1-1AA797A29E27}" name="Column3" dataDxfId="106"/>
-    <tableColumn id="4" xr3:uid="{CB82D336-531C-4BB2-AC91-1CAC6E92E6B7}" name="Column4" dataDxfId="105"/>
+    <tableColumn id="1" xr3:uid="{D1B206E0-BC18-44C3-AC3A-E386EBC240DA}" name="Column1" dataDxfId="129"/>
+    <tableColumn id="2" xr3:uid="{93DD1EAA-9879-4D36-9385-C9A727E59F3F}" name="Column2" dataDxfId="128"/>
+    <tableColumn id="3" xr3:uid="{C1074E65-5D51-4E3A-B9B1-1AA797A29E27}" name="Column3" dataDxfId="127"/>
+    <tableColumn id="4" xr3:uid="{CB82D336-531C-4BB2-AC91-1CAC6E92E6B7}" name="Column4" dataDxfId="126"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B1AE0DC9-D1F6-4E81-8D21-EBCF5F00B2B7}" name="Table262" displayName="Table262" ref="B7:H17" totalsRowShown="0" headerRowDxfId="104" dataDxfId="103" headerRowBorderDxfId="101" tableBorderDxfId="102" totalsRowBorderDxfId="100">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B1AE0DC9-D1F6-4E81-8D21-EBCF5F00B2B7}" name="Table262" displayName="Table262" ref="B7:H17" totalsRowShown="0" headerRowDxfId="125" dataDxfId="124" headerRowBorderDxfId="122" tableBorderDxfId="123" totalsRowBorderDxfId="121">
   <autoFilter ref="B7:H17" xr:uid="{B1AE0DC9-D1F6-4E81-8D21-EBCF5F00B2B7}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{C24C31E7-7289-4E64-B819-B73CBC38AAAC}" name="Resource Name" dataDxfId="99"/>
-    <tableColumn id="2" xr3:uid="{C2273D93-238B-4CCC-98AC-F0B06523F5CE}" name="In-progress" dataDxfId="98"/>
-    <tableColumn id="3" xr3:uid="{6E415DE6-A560-4988-877C-F716F699E312}" name="Done" dataDxfId="97"/>
-    <tableColumn id="4" xr3:uid="{C38A0EE9-47CE-4E5B-9C99-2B87137F78B9}" name="Discarded / Hold" dataDxfId="96"/>
-    <tableColumn id="5" xr3:uid="{1CC43B5C-77FA-4CED-8807-3E180A90E311}" name="Hours Spent - Project" dataDxfId="95"/>
-    <tableColumn id="6" xr3:uid="{356B8038-BBED-4F7F-B7BF-005E853F97B5}" name="Hours Spent - Non Project" dataDxfId="94"/>
-    <tableColumn id="7" xr3:uid="{AEE4776A-A2C0-4A70-ABAC-CB24A44ABC91}" name="Comments" dataDxfId="93"/>
+    <tableColumn id="1" xr3:uid="{C24C31E7-7289-4E64-B819-B73CBC38AAAC}" name="Resource Name" dataDxfId="120"/>
+    <tableColumn id="2" xr3:uid="{C2273D93-238B-4CCC-98AC-F0B06523F5CE}" name="In-progress" dataDxfId="119"/>
+    <tableColumn id="3" xr3:uid="{6E415DE6-A560-4988-877C-F716F699E312}" name="Done" dataDxfId="118"/>
+    <tableColumn id="4" xr3:uid="{C38A0EE9-47CE-4E5B-9C99-2B87137F78B9}" name="Discarded / Hold" dataDxfId="117"/>
+    <tableColumn id="5" xr3:uid="{1CC43B5C-77FA-4CED-8807-3E180A90E311}" name="Hours Spent - Project" dataDxfId="116"/>
+    <tableColumn id="6" xr3:uid="{356B8038-BBED-4F7F-B7BF-005E853F97B5}" name="Hours Spent - Non Project" dataDxfId="115"/>
+    <tableColumn id="7" xr3:uid="{AEE4776A-A2C0-4A70-ABAC-CB24A44ABC91}" name="Comments" dataDxfId="114"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ACFFF651-B126-4B94-92B4-F3166A18744A}" name="Table375" displayName="Table375" ref="B2:E4" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91" headerRowBorderDxfId="89" tableBorderDxfId="90" totalsRowBorderDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ACFFF651-B126-4B94-92B4-F3166A18744A}" name="Table375" displayName="Table375" ref="B2:E4" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112" headerRowBorderDxfId="110" tableBorderDxfId="111" totalsRowBorderDxfId="109">
   <autoFilter ref="B2:E4" xr:uid="{ACFFF651-B126-4B94-92B4-F3166A18744A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{83E614ED-6ABF-439F-A9B7-1518844696D4}" name="Column1" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{8840A839-8BBB-4DA6-9464-87D437F25D89}" name="Column2" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{ADAFE106-25BF-4F64-96D1-03AE2BD94818}" name="Column3" dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{377D3DE4-F5C8-4A2C-99F9-A46F41134437}" name="Column4" dataDxfId="84"/>
+    <tableColumn id="1" xr3:uid="{83E614ED-6ABF-439F-A9B7-1518844696D4}" name="Column1" dataDxfId="108"/>
+    <tableColumn id="2" xr3:uid="{8840A839-8BBB-4DA6-9464-87D437F25D89}" name="Column2" dataDxfId="107"/>
+    <tableColumn id="3" xr3:uid="{ADAFE106-25BF-4F64-96D1-03AE2BD94818}" name="Column3" dataDxfId="106"/>
+    <tableColumn id="4" xr3:uid="{377D3DE4-F5C8-4A2C-99F9-A46F41134437}" name="Column4" dataDxfId="105"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{A3D18560-C428-4868-B5CA-EBD1BE9F0FAE}" name="Table2621012" displayName="Table2621012" ref="B7:H17" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82" headerRowBorderDxfId="80" tableBorderDxfId="81" totalsRowBorderDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{A3D18560-C428-4868-B5CA-EBD1BE9F0FAE}" name="Table2621012" displayName="Table2621012" ref="B7:H17" totalsRowShown="0" headerRowDxfId="104" dataDxfId="103" headerRowBorderDxfId="101" tableBorderDxfId="102" totalsRowBorderDxfId="100">
   <autoFilter ref="B7:H17" xr:uid="{A30D6EFF-9BA6-4C4E-A49E-6E01C92313FC}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B99CA38C-6B70-44CB-94F1-34C0E18CAF38}" name="Resource Name" dataDxfId="78"/>
-    <tableColumn id="2" xr3:uid="{795625D3-DD18-4E77-8101-AB4369863885}" name="In-progress" dataDxfId="77"/>
-    <tableColumn id="3" xr3:uid="{F0C7DD64-C3AC-4A21-AA1F-AEAA2996C869}" name="Done" dataDxfId="76"/>
-    <tableColumn id="4" xr3:uid="{E1FC84EA-4ED4-4270-A149-E1E189A198C6}" name="Discarded / Hold" dataDxfId="75"/>
-    <tableColumn id="5" xr3:uid="{78CD14E8-1C2D-4CD1-A99E-E32FD07A85E3}" name="Hours Spent - Project" dataDxfId="74"/>
-    <tableColumn id="6" xr3:uid="{85ABF2B2-9FE1-4EFB-A748-B433E667EC67}" name="Hours Spent - Non Project" dataDxfId="73"/>
-    <tableColumn id="7" xr3:uid="{AA131BC6-5AD2-4A73-863A-093BE3A0E40F}" name="Comments" dataDxfId="72"/>
+    <tableColumn id="1" xr3:uid="{B99CA38C-6B70-44CB-94F1-34C0E18CAF38}" name="Resource Name" dataDxfId="99"/>
+    <tableColumn id="2" xr3:uid="{795625D3-DD18-4E77-8101-AB4369863885}" name="In-progress" dataDxfId="98"/>
+    <tableColumn id="3" xr3:uid="{F0C7DD64-C3AC-4A21-AA1F-AEAA2996C869}" name="Done" dataDxfId="97"/>
+    <tableColumn id="4" xr3:uid="{E1FC84EA-4ED4-4270-A149-E1E189A198C6}" name="Discarded / Hold" dataDxfId="96"/>
+    <tableColumn id="5" xr3:uid="{78CD14E8-1C2D-4CD1-A99E-E32FD07A85E3}" name="Hours Spent - Project" dataDxfId="95"/>
+    <tableColumn id="6" xr3:uid="{85ABF2B2-9FE1-4EFB-A748-B433E667EC67}" name="Hours Spent - Non Project" dataDxfId="94"/>
+    <tableColumn id="7" xr3:uid="{AA131BC6-5AD2-4A73-863A-093BE3A0E40F}" name="Comments" dataDxfId="93"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8069,8 +8642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F34C89B-AD9F-4621-B8F8-86D1460206B9}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8382,4 +8955,323 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E0DB949-3C0B-4717-A9F2-71E6CFA73838}">
+  <dimension ref="A2:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" customWidth="1"/>
+    <col min="4" max="4" width="68.7109375" customWidth="1"/>
+    <col min="5" max="5" width="62.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" ht="41.25">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" ht="21">
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" ht="21">
+      <c r="B4" s="6"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" ht="21">
+      <c r="B5" s="4"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" ht="20.25">
+      <c r="B6" s="11"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="103.5">
+      <c r="A7" s="12"/>
+      <c r="B7" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="243.75" customHeight="1">
+      <c r="B8" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="35">
+        <v>1</v>
+      </c>
+      <c r="G8" s="35">
+        <v>4</v>
+      </c>
+      <c r="H8" s="23"/>
+    </row>
+    <row r="9" spans="1:8" ht="233.25" customHeight="1">
+      <c r="B9" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="35">
+        <v>5</v>
+      </c>
+      <c r="G9" s="35"/>
+      <c r="H9" s="24"/>
+    </row>
+    <row r="10" spans="1:8" ht="147" customHeight="1">
+      <c r="B10" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="35">
+        <v>5</v>
+      </c>
+      <c r="G10" s="35"/>
+      <c r="H10" s="24"/>
+    </row>
+    <row r="11" spans="1:8" ht="229.5" customHeight="1">
+      <c r="B11" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="35">
+        <v>4.5</v>
+      </c>
+      <c r="G11" s="35">
+        <v>0</v>
+      </c>
+      <c r="H11" s="25"/>
+    </row>
+    <row r="12" spans="1:8" ht="186.75" customHeight="1">
+      <c r="B12" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="35">
+        <v>1</v>
+      </c>
+      <c r="G12" s="35">
+        <v>3</v>
+      </c>
+      <c r="H12" s="25"/>
+    </row>
+    <row r="13" spans="1:8" ht="192" customHeight="1">
+      <c r="B13" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="D13" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="35">
+        <v>5</v>
+      </c>
+      <c r="G13" s="35">
+        <v>0</v>
+      </c>
+      <c r="H13" s="25"/>
+    </row>
+    <row r="14" spans="1:8" ht="197.25" customHeight="1">
+      <c r="B14" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="35">
+        <v>4</v>
+      </c>
+      <c r="G14" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="25"/>
+    </row>
+    <row r="15" spans="1:8" ht="196.5" customHeight="1">
+      <c r="B15" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="47" t="s">
+        <v>143</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="45">
+        <v>5</v>
+      </c>
+      <c r="G15" s="35">
+        <v>0</v>
+      </c>
+      <c r="H15" s="26"/>
+    </row>
+    <row r="16" spans="1:8" ht="197.25" customHeight="1">
+      <c r="B16" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>149</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>150</v>
+      </c>
+      <c r="F16" s="35">
+        <v>4</v>
+      </c>
+      <c r="G16" s="35">
+        <v>1</v>
+      </c>
+      <c r="H16" s="27"/>
+    </row>
+    <row r="17" spans="2:8" ht="273.75" customHeight="1">
+      <c r="B17" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>146</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="42">
+        <v>5.5</v>
+      </c>
+      <c r="G17" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Timesheet Updated - Sheik Fareeth h
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68499DDD-4B65-4B7B-93D5-562FAD6A96CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE0FB4D0-5546-4F6D-879F-A568832A87F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 3(06-04-2022)" sheetId="40" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="153">
   <si>
     <t>Column1</t>
   </si>
@@ -580,6 +580,14 @@
 2 hr - Angular (Data binding and Directives)
 2 hr - Typescript(Basic syntac, variables,Types and Operators)
 0.5 hr - HLD Sample Documentation - overall view</t>
+  </si>
+  <si>
+    <t>Typescript &amp; Angular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROJECT :
+Brain Storming with team - 1 hr                                              Prepared Services &amp; View Models - 1 hr                                Prepared HLD - 2 hr                                                                       Explored Basics of Typescript &amp; Angular - 1 hr               
+</t>
   </si>
   <si>
     <t>Angular</t>
@@ -8962,7 +8970,7 @@
   <dimension ref="A2:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9209,10 +9217,10 @@
         <v>31</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="D15" s="47" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="E15" s="35" t="s">
         <v>41</v>
@@ -9230,13 +9238,13 @@
         <v>34</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D16" s="44" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E16" s="35" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F16" s="35">
         <v>4</v>

</xml_diff>

<commit_message>
Updated Timesheet Aravindhan & Kumaresh
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71898C14-8E82-4591-8F97-FBFB2E4A8A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{17D9CD1D-A24F-4A2C-9092-2531AFD2B857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="159">
   <si>
     <t>Column1</t>
   </si>
@@ -582,6 +582,11 @@
 0.5 hr - HLD Sample Documentation - overall view</t>
   </si>
   <si>
+    <t>1 Hr : Brainstorming with team.
+1 Hr :JavaScript  (functions,strings,arrowmethods etc..)                                                                1 Hr 15 Mins:JavaScript
+1 Hr :Typescript(functions)                                                                 1hr:Exploring Angular(Overview,Components)</t>
+  </si>
+  <si>
     <t>1 hr-Brainstorming with team                                              2hr-working on Layout                                                           1hr-Explored on Angular                                                       1hr -Explored on Web API</t>
   </si>
   <si>
@@ -591,6 +596,11 @@
     <t xml:space="preserve">1 Hr: Brainstorming with Team
 1 Hr 30 mins : Designed Home Layout page 
 1 hr : Attented Review with Anitha                                    30 mins : Explored Typescript                                             1 Hr : Exploration on Angular         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1hr : Brainstorming with team
+1hr : Exploring Java Script (basic)                                                     
+1hr :Exploring Type Script (basic)                                   1hr:Exploring Angular(Basics)                                                1hr:Refined layout </t>
   </si>
   <si>
     <t>Have to explore more on Angular Concepts</t>
@@ -8987,8 +8997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E0DB949-3C0B-4717-A9F2-71E6CFA73838}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9095,7 +9105,7 @@
         <v>131</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="E8" s="35" t="s">
         <v>41</v>
@@ -9104,7 +9114,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="35">
-        <v>4</v>
+        <v>4.25</v>
       </c>
       <c r="H8" s="23"/>
     </row>
@@ -9116,7 +9126,7 @@
         <v>113</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E9" s="35" t="s">
         <v>41</v>
@@ -9132,10 +9142,10 @@
         <v>20</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E10" s="35" t="s">
         <v>41</v>
@@ -9177,13 +9187,13 @@
         <v>138</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="E12" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F12" s="35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" s="35">
         <v>3</v>
@@ -9195,10 +9205,10 @@
         <v>27</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D13" s="44" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>41</v>
@@ -9237,10 +9247,10 @@
         <v>31</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D15" s="47" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E15" s="35" t="s">
         <v>41</v>
@@ -9258,10 +9268,10 @@
         <v>34</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D16" s="44" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E16" s="35"/>
       <c r="F16" s="35">

</xml_diff>

<commit_message>
Updated timesheet - Vinoth J
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BCCF76E-3408-4E34-971A-F87F0C4E5150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{53CDF53E-B7FC-4D60-B07F-661AE915FC39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 3(06-04-2022)" sheetId="40" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Day 9 (13-04-2022)" sheetId="45" r:id="rId7"/>
     <sheet name="Day10 ( 18-04-2022 )" sheetId="49" r:id="rId8"/>
     <sheet name="Day11 ( 19-04-2022 )" sheetId="51" r:id="rId9"/>
+    <sheet name="Day12 ( 20-04-2022 )" sheetId="52" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="166">
   <si>
     <t>Column1</t>
   </si>
@@ -634,12 +635,12 @@
 </t>
   </si>
   <si>
-    <t>Angular</t>
-  </si>
-  <si>
-    <t>1 hr : Brainstorming
+    <t>Exploring Angular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 hr : Brainstorming
 2 hr : exploration on angular basics
-1 hr : exploration on entity framework                              1 hr : exploration on angular components                       1 hr : Attented Review  with Anitha</t>
+1 hr : exploration on entity framework                              1 hr : exploration on angular components                       1 hr : Attented Review  with Anitha                                        1 hr : Explored typescript </t>
   </si>
   <si>
     <t xml:space="preserve">OVERVIEWING HLD </t>
@@ -650,6 +651,14 @@
 1 hr : Angular(Pipes,Dependency Injection,components recall,services)
 1 hr : Web API (RESTful services)
 1 hr : Typescript (static typing, interfaces)</t>
+  </si>
+  <si>
+    <t>Exploring angular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 hr : Brainstorming
+1 hr : Softskills
+1 hr : exploration on typescript(Loops)    </t>
   </si>
 </sst>
 </file>
@@ -1057,7 +1066,539 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="189">
+  <dxfs count="210">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="16"/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="16"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -5860,261 +6401,290 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B59126C7-EF4B-42B8-885B-D999B591F622}" name="Table2" displayName="Table2" ref="B9:H19" totalsRowShown="0" headerRowDxfId="188" dataDxfId="187" headerRowBorderDxfId="185" tableBorderDxfId="186" totalsRowBorderDxfId="184">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B59126C7-EF4B-42B8-885B-D999B591F622}" name="Table2" displayName="Table2" ref="B9:H19" totalsRowShown="0" headerRowDxfId="209" dataDxfId="208" headerRowBorderDxfId="206" tableBorderDxfId="207" totalsRowBorderDxfId="205">
   <autoFilter ref="B9:H19" xr:uid="{B59126C7-EF4B-42B8-885B-D999B591F622}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{52B5F38B-ABB3-47C0-BB3D-A29F2DE51CC7}" name="Resource Name" dataDxfId="183"/>
-    <tableColumn id="2" xr3:uid="{EE1FCD6C-E5A0-4CCC-B385-C1EFECE5FDAA}" name="In-progress" dataDxfId="182"/>
-    <tableColumn id="3" xr3:uid="{181E4433-047B-4DE4-8CA4-63F4C195E21B}" name="Done" dataDxfId="181"/>
-    <tableColumn id="4" xr3:uid="{3D6F0A13-3C98-4A4C-A37F-39C4F130B0FD}" name="Discarded / Hold" dataDxfId="180"/>
-    <tableColumn id="5" xr3:uid="{6C95647F-EC05-4637-9771-13884C172508}" name="Hours Spent - Project" dataDxfId="179"/>
-    <tableColumn id="6" xr3:uid="{61429939-C632-43F5-B197-7173C32B4F6F}" name="Hours Spent - Non Project" dataDxfId="178"/>
-    <tableColumn id="7" xr3:uid="{FA348B8C-B11C-46EA-A9B6-9E454AA967AA}" name="Comments" dataDxfId="177"/>
+    <tableColumn id="1" xr3:uid="{52B5F38B-ABB3-47C0-BB3D-A29F2DE51CC7}" name="Resource Name" dataDxfId="204"/>
+    <tableColumn id="2" xr3:uid="{EE1FCD6C-E5A0-4CCC-B385-C1EFECE5FDAA}" name="In-progress" dataDxfId="203"/>
+    <tableColumn id="3" xr3:uid="{181E4433-047B-4DE4-8CA4-63F4C195E21B}" name="Done" dataDxfId="202"/>
+    <tableColumn id="4" xr3:uid="{3D6F0A13-3C98-4A4C-A37F-39C4F130B0FD}" name="Discarded / Hold" dataDxfId="201"/>
+    <tableColumn id="5" xr3:uid="{6C95647F-EC05-4637-9771-13884C172508}" name="Hours Spent - Project" dataDxfId="200"/>
+    <tableColumn id="6" xr3:uid="{61429939-C632-43F5-B197-7173C32B4F6F}" name="Hours Spent - Non Project" dataDxfId="199"/>
+    <tableColumn id="7" xr3:uid="{FA348B8C-B11C-46EA-A9B6-9E454AA967AA}" name="Comments" dataDxfId="198"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D14697CD-D871-4BE9-9957-83E5498C6EE5}" name="Table3751113" displayName="Table3751113" ref="B2:E4" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91" headerRowBorderDxfId="89" tableBorderDxfId="90" totalsRowBorderDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D14697CD-D871-4BE9-9957-83E5498C6EE5}" name="Table3751113" displayName="Table3751113" ref="B2:E4" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112" headerRowBorderDxfId="110" tableBorderDxfId="111" totalsRowBorderDxfId="109">
   <autoFilter ref="B2:E4" xr:uid="{9D11D6AC-943D-4BD1-9800-DECD246F6E62}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{597AD08F-5CEE-486B-928A-4E0143DEB21C}" name="Column1" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{80BDA1F7-DDA4-494F-BB7E-61D9A6E30A98}" name="Column2" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{DF109DE4-28E3-4BB2-997F-34A3F319520E}" name="Column3" dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{C98D2CDB-0DA6-4DBC-80D8-197F6DC8262F}" name="Column4" dataDxfId="84"/>
+    <tableColumn id="1" xr3:uid="{597AD08F-5CEE-486B-928A-4E0143DEB21C}" name="Column1" dataDxfId="108"/>
+    <tableColumn id="2" xr3:uid="{80BDA1F7-DDA4-494F-BB7E-61D9A6E30A98}" name="Column2" dataDxfId="107"/>
+    <tableColumn id="3" xr3:uid="{DF109DE4-28E3-4BB2-997F-34A3F319520E}" name="Column3" dataDxfId="106"/>
+    <tableColumn id="4" xr3:uid="{C98D2CDB-0DA6-4DBC-80D8-197F6DC8262F}" name="Column4" dataDxfId="105"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{A036296C-A09A-4538-8AEF-52AAB9228500}" name="Table2621014" displayName="Table2621014" ref="B7:H17" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82" headerRowBorderDxfId="80" tableBorderDxfId="81" totalsRowBorderDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{A036296C-A09A-4538-8AEF-52AAB9228500}" name="Table2621014" displayName="Table2621014" ref="B7:H17" totalsRowShown="0" headerRowDxfId="104" dataDxfId="103" headerRowBorderDxfId="101" tableBorderDxfId="102" totalsRowBorderDxfId="100">
   <autoFilter ref="B7:H17" xr:uid="{A30D6EFF-9BA6-4C4E-A49E-6E01C92313FC}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{AF106EC2-9249-449D-84E6-7F225A50644A}" name="Resource Name" dataDxfId="78"/>
-    <tableColumn id="2" xr3:uid="{C5721F56-75DD-416B-8AF4-882B78C097A4}" name="In-progress" dataDxfId="77"/>
-    <tableColumn id="3" xr3:uid="{65371F98-F64C-4B19-8CA2-7EF266D44FBF}" name="Done" dataDxfId="76"/>
-    <tableColumn id="4" xr3:uid="{EDCBD646-6D4A-4D8E-A78F-13A92C55A829}" name="Discarded / Hold" dataDxfId="75"/>
-    <tableColumn id="5" xr3:uid="{5216518A-9337-493A-8FBE-8BB58C828250}" name="Hours Spent - Project" dataDxfId="74"/>
-    <tableColumn id="6" xr3:uid="{249FD4AA-FDB0-40B3-A254-56EFA2226474}" name="Hours Spent - Non Project" dataDxfId="73"/>
-    <tableColumn id="7" xr3:uid="{47669AF2-CA1E-4E4D-8758-1BE493ED8AF4}" name="Comments" dataDxfId="72"/>
+    <tableColumn id="1" xr3:uid="{AF106EC2-9249-449D-84E6-7F225A50644A}" name="Resource Name" dataDxfId="99"/>
+    <tableColumn id="2" xr3:uid="{C5721F56-75DD-416B-8AF4-882B78C097A4}" name="In-progress" dataDxfId="98"/>
+    <tableColumn id="3" xr3:uid="{65371F98-F64C-4B19-8CA2-7EF266D44FBF}" name="Done" dataDxfId="97"/>
+    <tableColumn id="4" xr3:uid="{EDCBD646-6D4A-4D8E-A78F-13A92C55A829}" name="Discarded / Hold" dataDxfId="96"/>
+    <tableColumn id="5" xr3:uid="{5216518A-9337-493A-8FBE-8BB58C828250}" name="Hours Spent - Project" dataDxfId="95"/>
+    <tableColumn id="6" xr3:uid="{249FD4AA-FDB0-40B3-A254-56EFA2226474}" name="Hours Spent - Non Project" dataDxfId="94"/>
+    <tableColumn id="7" xr3:uid="{47669AF2-CA1E-4E4D-8758-1BE493ED8AF4}" name="Comments" dataDxfId="93"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{7FA1E999-6830-41E9-8136-B3DD83876559}" name="Table3751115" displayName="Table3751115" ref="B2:E4" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70" headerRowBorderDxfId="68" tableBorderDxfId="69" totalsRowBorderDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{7FA1E999-6830-41E9-8136-B3DD83876559}" name="Table3751115" displayName="Table3751115" ref="B2:E4" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91" headerRowBorderDxfId="89" tableBorderDxfId="90" totalsRowBorderDxfId="88">
   <autoFilter ref="B2:E4" xr:uid="{9D11D6AC-943D-4BD1-9800-DECD246F6E62}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D67A75C6-50A5-4ED9-9562-707A5D717E14}" name="Column1" dataDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{4CBEA24E-4C4B-4B23-85EB-4A8217A30752}" name="Column2" dataDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{A13B37EF-4736-411C-BF75-CBDF316BAB90}" name="Column3" dataDxfId="64"/>
-    <tableColumn id="4" xr3:uid="{504EFC7F-2F49-4D22-ACB4-DCD4F1C95FE1}" name="Column4" dataDxfId="63"/>
+    <tableColumn id="1" xr3:uid="{D67A75C6-50A5-4ED9-9562-707A5D717E14}" name="Column1" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{4CBEA24E-4C4B-4B23-85EB-4A8217A30752}" name="Column2" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{A13B37EF-4736-411C-BF75-CBDF316BAB90}" name="Column3" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{504EFC7F-2F49-4D22-ACB4-DCD4F1C95FE1}" name="Column4" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A30D6EFF-9BA6-4C4E-A49E-6E01C92313FC}" name="Table26210" displayName="Table26210" ref="B7:H17" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61" headerRowBorderDxfId="59" tableBorderDxfId="60" totalsRowBorderDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A30D6EFF-9BA6-4C4E-A49E-6E01C92313FC}" name="Table26210" displayName="Table26210" ref="B7:H17" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82" headerRowBorderDxfId="80" tableBorderDxfId="81" totalsRowBorderDxfId="79">
   <autoFilter ref="B7:H17" xr:uid="{A30D6EFF-9BA6-4C4E-A49E-6E01C92313FC}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{CB514E32-07C5-40CB-B6EC-7CE1D7B57BF0}" name="Resource Name" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{C46C6E29-0824-4E17-8EAF-64A911996B4D}" name="In-progress" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{6B5DC81A-7A98-4BF7-864C-E5A79BB97505}" name="Done" dataDxfId="55"/>
-    <tableColumn id="4" xr3:uid="{0C243582-3F95-4A38-8545-76DB2898625E}" name="Discarded / Hold" dataDxfId="54"/>
-    <tableColumn id="5" xr3:uid="{FD3CD380-CAB0-422C-8CF7-6944378DDBE6}" name="Hours Spent - Project" dataDxfId="53"/>
-    <tableColumn id="6" xr3:uid="{145CB7BA-3D9C-44AC-9E51-716B58B77D2F}" name="Hours Spent - Non Project" dataDxfId="52"/>
-    <tableColumn id="7" xr3:uid="{507AE42A-A1CC-4934-90C2-3BFCE53238B3}" name="Comments" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{CB514E32-07C5-40CB-B6EC-7CE1D7B57BF0}" name="Resource Name" dataDxfId="78"/>
+    <tableColumn id="2" xr3:uid="{C46C6E29-0824-4E17-8EAF-64A911996B4D}" name="In-progress" dataDxfId="77"/>
+    <tableColumn id="3" xr3:uid="{6B5DC81A-7A98-4BF7-864C-E5A79BB97505}" name="Done" dataDxfId="76"/>
+    <tableColumn id="4" xr3:uid="{0C243582-3F95-4A38-8545-76DB2898625E}" name="Discarded / Hold" dataDxfId="75"/>
+    <tableColumn id="5" xr3:uid="{FD3CD380-CAB0-422C-8CF7-6944378DDBE6}" name="Hours Spent - Project" dataDxfId="74"/>
+    <tableColumn id="6" xr3:uid="{145CB7BA-3D9C-44AC-9E51-716B58B77D2F}" name="Hours Spent - Non Project" dataDxfId="73"/>
+    <tableColumn id="7" xr3:uid="{507AE42A-A1CC-4934-90C2-3BFCE53238B3}" name="Comments" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9D11D6AC-943D-4BD1-9800-DECD246F6E62}" name="Table37511" displayName="Table37511" ref="B2:E4" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49" headerRowBorderDxfId="47" tableBorderDxfId="48" totalsRowBorderDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9D11D6AC-943D-4BD1-9800-DECD246F6E62}" name="Table37511" displayName="Table37511" ref="B2:E4" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70" headerRowBorderDxfId="68" tableBorderDxfId="69" totalsRowBorderDxfId="67">
   <autoFilter ref="B2:E4" xr:uid="{9D11D6AC-943D-4BD1-9800-DECD246F6E62}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6B075576-4726-42C8-996A-A7B4B187D27F}" name="Column1" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{2B0F43B9-480B-4C54-A4CC-3DFC00711929}" name="Column2" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{4353F121-13EC-4653-AB7A-C0BBED71F612}" name="Column3" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{AD8279C5-6226-4ECF-A6C8-F9C70974EABE}" name="Column4" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{6B075576-4726-42C8-996A-A7B4B187D27F}" name="Column1" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{2B0F43B9-480B-4C54-A4CC-3DFC00711929}" name="Column2" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{4353F121-13EC-4653-AB7A-C0BBED71F612}" name="Column3" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{AD8279C5-6226-4ECF-A6C8-F9C70974EABE}" name="Column4" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{1356D4E1-15F0-41BF-B0C4-E4DC18B96A83}" name="Table2621016" displayName="Table2621016" ref="B7:H17" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" headerRowBorderDxfId="38" tableBorderDxfId="39" totalsRowBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{1356D4E1-15F0-41BF-B0C4-E4DC18B96A83}" name="Table2621016" displayName="Table2621016" ref="B7:H17" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61" headerRowBorderDxfId="59" tableBorderDxfId="60" totalsRowBorderDxfId="58">
   <autoFilter ref="B7:H17" xr:uid="{1356D4E1-15F0-41BF-B0C4-E4DC18B96A83}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{975CF6D7-F24C-4D9F-BA9F-439AF60EF114}" name="Resource Name" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{BC36331B-5C09-49F2-8E13-D5168DD28D0F}" name="In-progress" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{41B5A763-B80D-4E4B-976F-9969D2C0C14F}" name="Done" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{5D1F40BB-F239-4A1D-AEF6-82A5FC99D7CD}" name="Discarded / Hold" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{5C9549F2-9CF2-45B7-98E8-1D291B3630B2}" name="Hours Spent - Project" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{04DC6A6C-EEB6-4EF4-911D-C37E2C5B40FF}" name="Hours Spent - Non Project" dataDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{C3902E87-CCB6-47C9-9BC1-FD0B37543238}" name="Comments" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{975CF6D7-F24C-4D9F-BA9F-439AF60EF114}" name="Resource Name" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{BC36331B-5C09-49F2-8E13-D5168DD28D0F}" name="In-progress" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{41B5A763-B80D-4E4B-976F-9969D2C0C14F}" name="Done" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{5D1F40BB-F239-4A1D-AEF6-82A5FC99D7CD}" name="Discarded / Hold" dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{5C9549F2-9CF2-45B7-98E8-1D291B3630B2}" name="Hours Spent - Project" dataDxfId="53"/>
+    <tableColumn id="6" xr3:uid="{04DC6A6C-EEB6-4EF4-911D-C37E2C5B40FF}" name="Hours Spent - Non Project" dataDxfId="52"/>
+    <tableColumn id="7" xr3:uid="{C3902E87-CCB6-47C9-9BC1-FD0B37543238}" name="Comments" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E3497E54-1E59-44E7-9480-106E98FB838A}" name="Table3751117" displayName="Table3751117" ref="B2:E4" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" headerRowBorderDxfId="26" tableBorderDxfId="27" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E3497E54-1E59-44E7-9480-106E98FB838A}" name="Table3751117" displayName="Table3751117" ref="B2:E4" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49" headerRowBorderDxfId="47" tableBorderDxfId="48" totalsRowBorderDxfId="46">
   <autoFilter ref="B2:E4" xr:uid="{E3497E54-1E59-44E7-9480-106E98FB838A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{69E7B7B7-0FF3-43D1-AE4A-578CB3CCCFBD}" name="Column1" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{753FC1E8-1B96-4804-A794-92A8953D5EE2}" name="Column2" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{50B38A4B-BAF8-4640-8ECB-0900A6C915DB}" name="Column3" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{4432DCD0-98FF-4B59-BAB7-E3FE0A3EDFBC}" name="Column4" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{69E7B7B7-0FF3-43D1-AE4A-578CB3CCCFBD}" name="Column1" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{753FC1E8-1B96-4804-A794-92A8953D5EE2}" name="Column2" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{50B38A4B-BAF8-4640-8ECB-0900A6C915DB}" name="Column3" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{4432DCD0-98FF-4B59-BAB7-E3FE0A3EDFBC}" name="Column4" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{D3490739-1854-4802-BC7E-8F8A56938939}" name="Table262101618" displayName="Table262101618" ref="B7:H17" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{D3490739-1854-4802-BC7E-8F8A56938939}" name="Table262101618" displayName="Table262101618" ref="B7:H17" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" headerRowBorderDxfId="38" tableBorderDxfId="39" totalsRowBorderDxfId="37">
   <autoFilter ref="B7:H17" xr:uid="{1356D4E1-15F0-41BF-B0C4-E4DC18B96A83}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F4CDC508-938F-4C7B-9D78-6C7897C95C75}" name="Resource Name" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{D24B5720-9179-4EA6-A1B2-11FFE3971AE0}" name="In-progress" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{38376D7D-1777-43ED-87F4-271C7CA93BC0}" name="Done" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{27CF804E-18A7-4ED9-9891-7FE4B93C6D6C}" name="Discarded / Hold" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{F23FF8B6-B301-4C5F-ACF3-3D16EEFFC3F0}" name="Hours Spent - Project" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{2D0142DB-38B6-4D6B-A60F-A9A19574C7ED}" name="Hours Spent - Non Project" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{8BAC7AAB-A572-4256-AFEE-71DC94CC59B9}" name="Comments" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{F4CDC508-938F-4C7B-9D78-6C7897C95C75}" name="Resource Name" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{D24B5720-9179-4EA6-A1B2-11FFE3971AE0}" name="In-progress" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{38376D7D-1777-43ED-87F4-271C7CA93BC0}" name="Done" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{27CF804E-18A7-4ED9-9891-7FE4B93C6D6C}" name="Discarded / Hold" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{F23FF8B6-B301-4C5F-ACF3-3D16EEFFC3F0}" name="Hours Spent - Project" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{2D0142DB-38B6-4D6B-A60F-A9A19574C7ED}" name="Hours Spent - Non Project" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{8BAC7AAB-A572-4256-AFEE-71DC94CC59B9}" name="Comments" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{65B9F601-45A2-418D-921A-3D56A32B6C21}" name="Table375111719" displayName="Table375111719" ref="B2:E4" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{65B9F601-45A2-418D-921A-3D56A32B6C21}" name="Table375111719" displayName="Table375111719" ref="B2:E4" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" headerRowBorderDxfId="26" tableBorderDxfId="27" totalsRowBorderDxfId="25">
   <autoFilter ref="B2:E4" xr:uid="{E3497E54-1E59-44E7-9480-106E98FB838A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6E252E52-03A5-4570-990A-B3378296E039}" name="Column1" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{D5447885-EF1E-44FE-B1A4-EE1475056221}" name="Column2" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{2F816DC6-3307-4F6E-9962-EB8AB2F91C9F}" name="Column3" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{21AE6030-4E77-45A3-8CDA-342E87194417}" name="Column4" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{6E252E52-03A5-4570-990A-B3378296E039}" name="Column1" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{D5447885-EF1E-44FE-B1A4-EE1475056221}" name="Column2" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{2F816DC6-3307-4F6E-9962-EB8AB2F91C9F}" name="Column3" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{21AE6030-4E77-45A3-8CDA-342E87194417}" name="Column4" dataDxfId="21"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{567599D8-F2AC-4863-A31E-867E4662A188}" name="Table26210161820" displayName="Table26210161820" ref="B7:H17" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+  <autoFilter ref="B7:H17" xr:uid="{1356D4E1-15F0-41BF-B0C4-E4DC18B96A83}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{6862ACD5-06E8-4C76-86B8-0FBF46C719AB}" name="Resource Name" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{2FEAF882-A5EF-4611-91BB-CAEDE2BD0142}" name="In-progress" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{FB3D921D-555F-47F7-9140-AB8143CB71BA}" name="Done" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{BD8867CA-8566-48C2-BDB8-839066AC235A}" name="Discarded / Hold" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{F71E5005-E794-436C-8ABB-93D21EB0BD11}" name="Hours Spent - Project" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{53117683-12E5-4475-8EE2-ECA8DBFEEF45}" name="Hours Spent - Non Project" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{A1C72867-09F6-497F-ACF5-1458D252B64F}" name="Comments" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BF3C43CE-B630-4202-BD3A-6EE2D770899A}" name="Table3" displayName="Table3" ref="B4:E6" totalsRowShown="0" headerRowDxfId="176" dataDxfId="175" headerRowBorderDxfId="173" tableBorderDxfId="174" totalsRowBorderDxfId="172">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BF3C43CE-B630-4202-BD3A-6EE2D770899A}" name="Table3" displayName="Table3" ref="B4:E6" totalsRowShown="0" headerRowDxfId="197" dataDxfId="196" headerRowBorderDxfId="194" tableBorderDxfId="195" totalsRowBorderDxfId="193">
   <autoFilter ref="B4:E6" xr:uid="{BF3C43CE-B630-4202-BD3A-6EE2D770899A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BE43EB49-4D5D-488E-9520-6CE4AC2E5C1B}" name="Column1" dataDxfId="171"/>
-    <tableColumn id="2" xr3:uid="{16DFD0E6-4C5E-443C-BF24-706A867EF798}" name="Column2" dataDxfId="170"/>
-    <tableColumn id="3" xr3:uid="{DC8A145E-C833-4BE6-BAE5-7E5E2AC2891C}" name="Column3" dataDxfId="169"/>
-    <tableColumn id="4" xr3:uid="{9454D612-74D7-428F-B9A0-7151862F7C2A}" name="Column4" dataDxfId="168"/>
+    <tableColumn id="1" xr3:uid="{BE43EB49-4D5D-488E-9520-6CE4AC2E5C1B}" name="Column1" dataDxfId="192"/>
+    <tableColumn id="2" xr3:uid="{16DFD0E6-4C5E-443C-BF24-706A867EF798}" name="Column2" dataDxfId="191"/>
+    <tableColumn id="3" xr3:uid="{DC8A145E-C833-4BE6-BAE5-7E5E2AC2891C}" name="Column3" dataDxfId="190"/>
+    <tableColumn id="4" xr3:uid="{9454D612-74D7-428F-B9A0-7151862F7C2A}" name="Column4" dataDxfId="189"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{3AB7E480-AA41-45EE-8BD2-799B66CF977F}" name="Table37511171921" displayName="Table37511171921" ref="B2:E4" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+  <autoFilter ref="B2:E4" xr:uid="{E3497E54-1E59-44E7-9480-106E98FB838A}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{5F5286EA-BF04-4F20-B734-0734EC625276}" name="Column1" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{2666153F-F4E8-45C3-9985-38E5471A82F0}" name="Column2" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{ED99E108-F673-4294-9E8D-A329582DF55B}" name="Column3" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{B0F02456-D0DE-4E93-9016-90FA89E16184}" name="Column4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{46BFD46F-1AD6-4EF9-9F4D-9841A6E71CD9}" name="Table26" displayName="Table26" ref="B8:H18" totalsRowShown="0" headerRowDxfId="167" dataDxfId="166" headerRowBorderDxfId="164" tableBorderDxfId="165" totalsRowBorderDxfId="163">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{46BFD46F-1AD6-4EF9-9F4D-9841A6E71CD9}" name="Table26" displayName="Table26" ref="B8:H18" totalsRowShown="0" headerRowDxfId="188" dataDxfId="187" headerRowBorderDxfId="185" tableBorderDxfId="186" totalsRowBorderDxfId="184">
   <autoFilter ref="B8:H18" xr:uid="{46BFD46F-1AD6-4EF9-9F4D-9841A6E71CD9}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{7428D5F6-9EE3-49C6-B1BE-E57BFF59C7B0}" name="Resource Name" dataDxfId="162"/>
-    <tableColumn id="2" xr3:uid="{8EF82413-9CDB-4809-98BD-913D08316031}" name="In-progress" dataDxfId="161"/>
-    <tableColumn id="3" xr3:uid="{B4E2F1CC-113D-4DBD-9D8F-AFFEF819725B}" name="Done" dataDxfId="160"/>
-    <tableColumn id="4" xr3:uid="{A8C1C667-3FF8-4B7C-AEC8-2DD543708DEA}" name="Discarded / Hold" dataDxfId="159"/>
-    <tableColumn id="5" xr3:uid="{DF5599B4-665D-4C1C-8DFF-80F68FB27D64}" name="Hours Spent - Project" dataDxfId="158"/>
-    <tableColumn id="6" xr3:uid="{EAD7742A-CE22-40A8-90BD-AB0C0555FA39}" name="Hours Spent - Non Project" dataDxfId="157"/>
-    <tableColumn id="7" xr3:uid="{52C2DA4C-9FFA-48AF-B36A-2837B9ED00F1}" name="Comments" dataDxfId="156"/>
+    <tableColumn id="1" xr3:uid="{7428D5F6-9EE3-49C6-B1BE-E57BFF59C7B0}" name="Resource Name" dataDxfId="183"/>
+    <tableColumn id="2" xr3:uid="{8EF82413-9CDB-4809-98BD-913D08316031}" name="In-progress" dataDxfId="182"/>
+    <tableColumn id="3" xr3:uid="{B4E2F1CC-113D-4DBD-9D8F-AFFEF819725B}" name="Done" dataDxfId="181"/>
+    <tableColumn id="4" xr3:uid="{A8C1C667-3FF8-4B7C-AEC8-2DD543708DEA}" name="Discarded / Hold" dataDxfId="180"/>
+    <tableColumn id="5" xr3:uid="{DF5599B4-665D-4C1C-8DFF-80F68FB27D64}" name="Hours Spent - Project" dataDxfId="179"/>
+    <tableColumn id="6" xr3:uid="{EAD7742A-CE22-40A8-90BD-AB0C0555FA39}" name="Hours Spent - Non Project" dataDxfId="178"/>
+    <tableColumn id="7" xr3:uid="{52C2DA4C-9FFA-48AF-B36A-2837B9ED00F1}" name="Comments" dataDxfId="177"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9997EBAF-6A71-418E-B851-C8B1915211B5}" name="Table37" displayName="Table37" ref="B3:E5" totalsRowShown="0" headerRowDxfId="155" dataDxfId="154" headerRowBorderDxfId="152" tableBorderDxfId="153" totalsRowBorderDxfId="151">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9997EBAF-6A71-418E-B851-C8B1915211B5}" name="Table37" displayName="Table37" ref="B3:E5" totalsRowShown="0" headerRowDxfId="176" dataDxfId="175" headerRowBorderDxfId="173" tableBorderDxfId="174" totalsRowBorderDxfId="172">
   <autoFilter ref="B3:E5" xr:uid="{9997EBAF-6A71-418E-B851-C8B1915211B5}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{7EDDA488-2881-4A15-9B9C-777D834D815F}" name="Column1" dataDxfId="150"/>
-    <tableColumn id="2" xr3:uid="{AFE02A3A-062D-4251-90A2-DA5D33B35508}" name="Column2" dataDxfId="149"/>
-    <tableColumn id="3" xr3:uid="{ED8EDBC8-15CC-4013-9D78-2DF925F82DCD}" name="Column3" dataDxfId="148"/>
-    <tableColumn id="4" xr3:uid="{62C95B61-46F3-42F7-A1B8-B69D37DD10DF}" name="Column4" dataDxfId="147"/>
+    <tableColumn id="1" xr3:uid="{7EDDA488-2881-4A15-9B9C-777D834D815F}" name="Column1" dataDxfId="171"/>
+    <tableColumn id="2" xr3:uid="{AFE02A3A-062D-4251-90A2-DA5D33B35508}" name="Column2" dataDxfId="170"/>
+    <tableColumn id="3" xr3:uid="{ED8EDBC8-15CC-4013-9D78-2DF925F82DCD}" name="Column3" dataDxfId="169"/>
+    <tableColumn id="4" xr3:uid="{62C95B61-46F3-42F7-A1B8-B69D37DD10DF}" name="Column4" dataDxfId="168"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{158FF28A-C282-456C-9B5E-C00624BAAA83}" name="Table2628" displayName="Table2628" ref="B7:H17" totalsRowShown="0" headerRowDxfId="146" dataDxfId="145" headerRowBorderDxfId="143" tableBorderDxfId="144" totalsRowBorderDxfId="142">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{158FF28A-C282-456C-9B5E-C00624BAAA83}" name="Table2628" displayName="Table2628" ref="B7:H17" totalsRowShown="0" headerRowDxfId="167" dataDxfId="166" headerRowBorderDxfId="164" tableBorderDxfId="165" totalsRowBorderDxfId="163">
   <autoFilter ref="B7:H17" xr:uid="{B1AE0DC9-D1F6-4E81-8D21-EBCF5F00B2B7}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{FA7FB678-9F12-498D-AC8C-EA3804FA6C35}" name="Resource Name" dataDxfId="141"/>
-    <tableColumn id="2" xr3:uid="{393B2B95-8815-4457-B760-B5E70FBBB0A5}" name="In-progress" dataDxfId="140"/>
-    <tableColumn id="3" xr3:uid="{400FD95F-D628-4B07-904B-1F5E11C584A9}" name="Done" dataDxfId="139"/>
-    <tableColumn id="4" xr3:uid="{DA6CAF01-4620-4AD9-8F22-C26934025345}" name="Discarded / Hold" dataDxfId="138"/>
-    <tableColumn id="5" xr3:uid="{D70C3DC4-AF79-4EA9-916E-2DDB8181B077}" name="Hours Spent - Project" dataDxfId="137"/>
-    <tableColumn id="6" xr3:uid="{BA92211F-9DF3-4897-86C0-5FE2D8FC9C28}" name="Hours Spent - Non Project" dataDxfId="136"/>
-    <tableColumn id="7" xr3:uid="{673B654E-8412-4BCE-9293-22370300F740}" name="Comments" dataDxfId="135"/>
+    <tableColumn id="1" xr3:uid="{FA7FB678-9F12-498D-AC8C-EA3804FA6C35}" name="Resource Name" dataDxfId="162"/>
+    <tableColumn id="2" xr3:uid="{393B2B95-8815-4457-B760-B5E70FBBB0A5}" name="In-progress" dataDxfId="161"/>
+    <tableColumn id="3" xr3:uid="{400FD95F-D628-4B07-904B-1F5E11C584A9}" name="Done" dataDxfId="160"/>
+    <tableColumn id="4" xr3:uid="{DA6CAF01-4620-4AD9-8F22-C26934025345}" name="Discarded / Hold" dataDxfId="159"/>
+    <tableColumn id="5" xr3:uid="{D70C3DC4-AF79-4EA9-916E-2DDB8181B077}" name="Hours Spent - Project" dataDxfId="158"/>
+    <tableColumn id="6" xr3:uid="{BA92211F-9DF3-4897-86C0-5FE2D8FC9C28}" name="Hours Spent - Non Project" dataDxfId="157"/>
+    <tableColumn id="7" xr3:uid="{673B654E-8412-4BCE-9293-22370300F740}" name="Comments" dataDxfId="156"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FE979438-BC3B-45D4-9D8F-CD3DAC132734}" name="Table3759" displayName="Table3759" ref="B2:E4" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133" headerRowBorderDxfId="131" tableBorderDxfId="132" totalsRowBorderDxfId="130">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FE979438-BC3B-45D4-9D8F-CD3DAC132734}" name="Table3759" displayName="Table3759" ref="B2:E4" totalsRowShown="0" headerRowDxfId="155" dataDxfId="154" headerRowBorderDxfId="152" tableBorderDxfId="153" totalsRowBorderDxfId="151">
   <autoFilter ref="B2:E4" xr:uid="{ACFFF651-B126-4B94-92B4-F3166A18744A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D1B206E0-BC18-44C3-AC3A-E386EBC240DA}" name="Column1" dataDxfId="129"/>
-    <tableColumn id="2" xr3:uid="{93DD1EAA-9879-4D36-9385-C9A727E59F3F}" name="Column2" dataDxfId="128"/>
-    <tableColumn id="3" xr3:uid="{C1074E65-5D51-4E3A-B9B1-1AA797A29E27}" name="Column3" dataDxfId="127"/>
-    <tableColumn id="4" xr3:uid="{CB82D336-531C-4BB2-AC91-1CAC6E92E6B7}" name="Column4" dataDxfId="126"/>
+    <tableColumn id="1" xr3:uid="{D1B206E0-BC18-44C3-AC3A-E386EBC240DA}" name="Column1" dataDxfId="150"/>
+    <tableColumn id="2" xr3:uid="{93DD1EAA-9879-4D36-9385-C9A727E59F3F}" name="Column2" dataDxfId="149"/>
+    <tableColumn id="3" xr3:uid="{C1074E65-5D51-4E3A-B9B1-1AA797A29E27}" name="Column3" dataDxfId="148"/>
+    <tableColumn id="4" xr3:uid="{CB82D336-531C-4BB2-AC91-1CAC6E92E6B7}" name="Column4" dataDxfId="147"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B1AE0DC9-D1F6-4E81-8D21-EBCF5F00B2B7}" name="Table262" displayName="Table262" ref="B7:H17" totalsRowShown="0" headerRowDxfId="125" dataDxfId="124" headerRowBorderDxfId="122" tableBorderDxfId="123" totalsRowBorderDxfId="121">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B1AE0DC9-D1F6-4E81-8D21-EBCF5F00B2B7}" name="Table262" displayName="Table262" ref="B7:H17" totalsRowShown="0" headerRowDxfId="146" dataDxfId="145" headerRowBorderDxfId="143" tableBorderDxfId="144" totalsRowBorderDxfId="142">
   <autoFilter ref="B7:H17" xr:uid="{B1AE0DC9-D1F6-4E81-8D21-EBCF5F00B2B7}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{C24C31E7-7289-4E64-B819-B73CBC38AAAC}" name="Resource Name" dataDxfId="120"/>
-    <tableColumn id="2" xr3:uid="{C2273D93-238B-4CCC-98AC-F0B06523F5CE}" name="In-progress" dataDxfId="119"/>
-    <tableColumn id="3" xr3:uid="{6E415DE6-A560-4988-877C-F716F699E312}" name="Done" dataDxfId="118"/>
-    <tableColumn id="4" xr3:uid="{C38A0EE9-47CE-4E5B-9C99-2B87137F78B9}" name="Discarded / Hold" dataDxfId="117"/>
-    <tableColumn id="5" xr3:uid="{1CC43B5C-77FA-4CED-8807-3E180A90E311}" name="Hours Spent - Project" dataDxfId="116"/>
-    <tableColumn id="6" xr3:uid="{356B8038-BBED-4F7F-B7BF-005E853F97B5}" name="Hours Spent - Non Project" dataDxfId="115"/>
-    <tableColumn id="7" xr3:uid="{AEE4776A-A2C0-4A70-ABAC-CB24A44ABC91}" name="Comments" dataDxfId="114"/>
+    <tableColumn id="1" xr3:uid="{C24C31E7-7289-4E64-B819-B73CBC38AAAC}" name="Resource Name" dataDxfId="141"/>
+    <tableColumn id="2" xr3:uid="{C2273D93-238B-4CCC-98AC-F0B06523F5CE}" name="In-progress" dataDxfId="140"/>
+    <tableColumn id="3" xr3:uid="{6E415DE6-A560-4988-877C-F716F699E312}" name="Done" dataDxfId="139"/>
+    <tableColumn id="4" xr3:uid="{C38A0EE9-47CE-4E5B-9C99-2B87137F78B9}" name="Discarded / Hold" dataDxfId="138"/>
+    <tableColumn id="5" xr3:uid="{1CC43B5C-77FA-4CED-8807-3E180A90E311}" name="Hours Spent - Project" dataDxfId="137"/>
+    <tableColumn id="6" xr3:uid="{356B8038-BBED-4F7F-B7BF-005E853F97B5}" name="Hours Spent - Non Project" dataDxfId="136"/>
+    <tableColumn id="7" xr3:uid="{AEE4776A-A2C0-4A70-ABAC-CB24A44ABC91}" name="Comments" dataDxfId="135"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ACFFF651-B126-4B94-92B4-F3166A18744A}" name="Table375" displayName="Table375" ref="B2:E4" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112" headerRowBorderDxfId="110" tableBorderDxfId="111" totalsRowBorderDxfId="109">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ACFFF651-B126-4B94-92B4-F3166A18744A}" name="Table375" displayName="Table375" ref="B2:E4" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133" headerRowBorderDxfId="131" tableBorderDxfId="132" totalsRowBorderDxfId="130">
   <autoFilter ref="B2:E4" xr:uid="{ACFFF651-B126-4B94-92B4-F3166A18744A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{83E614ED-6ABF-439F-A9B7-1518844696D4}" name="Column1" dataDxfId="108"/>
-    <tableColumn id="2" xr3:uid="{8840A839-8BBB-4DA6-9464-87D437F25D89}" name="Column2" dataDxfId="107"/>
-    <tableColumn id="3" xr3:uid="{ADAFE106-25BF-4F64-96D1-03AE2BD94818}" name="Column3" dataDxfId="106"/>
-    <tableColumn id="4" xr3:uid="{377D3DE4-F5C8-4A2C-99F9-A46F41134437}" name="Column4" dataDxfId="105"/>
+    <tableColumn id="1" xr3:uid="{83E614ED-6ABF-439F-A9B7-1518844696D4}" name="Column1" dataDxfId="129"/>
+    <tableColumn id="2" xr3:uid="{8840A839-8BBB-4DA6-9464-87D437F25D89}" name="Column2" dataDxfId="128"/>
+    <tableColumn id="3" xr3:uid="{ADAFE106-25BF-4F64-96D1-03AE2BD94818}" name="Column3" dataDxfId="127"/>
+    <tableColumn id="4" xr3:uid="{377D3DE4-F5C8-4A2C-99F9-A46F41134437}" name="Column4" dataDxfId="126"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{A3D18560-C428-4868-B5CA-EBD1BE9F0FAE}" name="Table2621012" displayName="Table2621012" ref="B7:H17" totalsRowShown="0" headerRowDxfId="104" dataDxfId="103" headerRowBorderDxfId="101" tableBorderDxfId="102" totalsRowBorderDxfId="100">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{A3D18560-C428-4868-B5CA-EBD1BE9F0FAE}" name="Table2621012" displayName="Table2621012" ref="B7:H17" totalsRowShown="0" headerRowDxfId="125" dataDxfId="124" headerRowBorderDxfId="122" tableBorderDxfId="123" totalsRowBorderDxfId="121">
   <autoFilter ref="B7:H17" xr:uid="{A30D6EFF-9BA6-4C4E-A49E-6E01C92313FC}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B99CA38C-6B70-44CB-94F1-34C0E18CAF38}" name="Resource Name" dataDxfId="99"/>
-    <tableColumn id="2" xr3:uid="{795625D3-DD18-4E77-8101-AB4369863885}" name="In-progress" dataDxfId="98"/>
-    <tableColumn id="3" xr3:uid="{F0C7DD64-C3AC-4A21-AA1F-AEAA2996C869}" name="Done" dataDxfId="97"/>
-    <tableColumn id="4" xr3:uid="{E1FC84EA-4ED4-4270-A149-E1E189A198C6}" name="Discarded / Hold" dataDxfId="96"/>
-    <tableColumn id="5" xr3:uid="{78CD14E8-1C2D-4CD1-A99E-E32FD07A85E3}" name="Hours Spent - Project" dataDxfId="95"/>
-    <tableColumn id="6" xr3:uid="{85ABF2B2-9FE1-4EFB-A748-B433E667EC67}" name="Hours Spent - Non Project" dataDxfId="94"/>
-    <tableColumn id="7" xr3:uid="{AA131BC6-5AD2-4A73-863A-093BE3A0E40F}" name="Comments" dataDxfId="93"/>
+    <tableColumn id="1" xr3:uid="{B99CA38C-6B70-44CB-94F1-34C0E18CAF38}" name="Resource Name" dataDxfId="120"/>
+    <tableColumn id="2" xr3:uid="{795625D3-DD18-4E77-8101-AB4369863885}" name="In-progress" dataDxfId="119"/>
+    <tableColumn id="3" xr3:uid="{F0C7DD64-C3AC-4A21-AA1F-AEAA2996C869}" name="Done" dataDxfId="118"/>
+    <tableColumn id="4" xr3:uid="{E1FC84EA-4ED4-4270-A149-E1E189A198C6}" name="Discarded / Hold" dataDxfId="117"/>
+    <tableColumn id="5" xr3:uid="{78CD14E8-1C2D-4CD1-A99E-E32FD07A85E3}" name="Hours Spent - Project" dataDxfId="116"/>
+    <tableColumn id="6" xr3:uid="{85ABF2B2-9FE1-4EFB-A748-B433E667EC67}" name="Hours Spent - Non Project" dataDxfId="115"/>
+    <tableColumn id="7" xr3:uid="{AA131BC6-5AD2-4A73-863A-093BE3A0E40F}" name="Comments" dataDxfId="114"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6762,6 +7332,325 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9136D698-C624-4D52-A3F8-D913404DF880}">
+  <dimension ref="A2:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B15" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" customWidth="1"/>
+    <col min="4" max="4" width="68.7109375" customWidth="1"/>
+    <col min="5" max="5" width="62.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" ht="41.25">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" ht="21">
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" ht="21">
+      <c r="B4" s="6"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" ht="21">
+      <c r="B5" s="4"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" ht="20.25">
+      <c r="B6" s="11"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="103.5">
+      <c r="A7" s="12"/>
+      <c r="B7" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="243.75" customHeight="1">
+      <c r="B8" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="35">
+        <v>1</v>
+      </c>
+      <c r="G8" s="35">
+        <v>4.25</v>
+      </c>
+      <c r="H8" s="23"/>
+    </row>
+    <row r="9" spans="1:8" ht="233.25" customHeight="1">
+      <c r="B9" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="35">
+        <v>5</v>
+      </c>
+      <c r="G9" s="35"/>
+      <c r="H9" s="24"/>
+    </row>
+    <row r="10" spans="1:8" ht="147" customHeight="1">
+      <c r="B10" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>150</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="35">
+        <v>4</v>
+      </c>
+      <c r="G10" s="35">
+        <v>1</v>
+      </c>
+      <c r="H10" s="24"/>
+    </row>
+    <row r="11" spans="1:8" ht="229.5" customHeight="1">
+      <c r="B11" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="35">
+        <v>4</v>
+      </c>
+      <c r="G11" s="35">
+        <v>0</v>
+      </c>
+      <c r="H11" s="25"/>
+    </row>
+    <row r="12" spans="1:8" ht="186.75" customHeight="1">
+      <c r="B12" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="35">
+        <v>2</v>
+      </c>
+      <c r="G12" s="35">
+        <v>3</v>
+      </c>
+      <c r="H12" s="25"/>
+    </row>
+    <row r="13" spans="1:8" ht="192" customHeight="1">
+      <c r="B13" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="35">
+        <v>5</v>
+      </c>
+      <c r="G13" s="35">
+        <v>0</v>
+      </c>
+      <c r="H13" s="25"/>
+    </row>
+    <row r="14" spans="1:8" ht="197.25" customHeight="1">
+      <c r="B14" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="35">
+        <v>5</v>
+      </c>
+      <c r="G14" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="25"/>
+    </row>
+    <row r="15" spans="1:8" ht="196.5" customHeight="1">
+      <c r="B15" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="D15" s="47" t="s">
+        <v>159</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="45">
+        <v>5</v>
+      </c>
+      <c r="G15" s="35">
+        <v>0</v>
+      </c>
+      <c r="H15" s="26"/>
+    </row>
+    <row r="16" spans="1:8" ht="197.25" customHeight="1">
+      <c r="B16" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35">
+        <v>2</v>
+      </c>
+      <c r="G16" s="35">
+        <v>1</v>
+      </c>
+      <c r="H16" s="27"/>
+    </row>
+    <row r="17" spans="2:8" ht="273.75" customHeight="1">
+      <c r="B17" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="42">
+        <v>4</v>
+      </c>
+      <c r="G17" s="42">
+        <v>1</v>
+      </c>
+      <c r="H17" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8A9E40-E750-40E6-A7F8-FB6957E31B8C}">
   <dimension ref="A3:K21"/>
@@ -9020,8 +9909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E0DB949-3C0B-4717-A9F2-71E6CFA73838}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9298,7 +10187,7 @@
       </c>
       <c r="E16" s="35"/>
       <c r="F16" s="35">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16" s="35">
         <v>1</v>

</xml_diff>

<commit_message>
Updated Time Sheet - SheikFareeth H
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6042EF6-A1E5-42CD-BCBB-6C5BDD060728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{09528C0F-C103-4E0C-86DE-855C002F9649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="171">
   <si>
     <t>Column1</t>
   </si>
@@ -667,6 +667,11 @@
     <t xml:space="preserve">1 hour               :  Brainstorming with team
 1 hr                    :  Attended the soft skills session (Presentation on challenges faced in our life )
 1 hr                    : Exploring on javascript and typescript execises.                                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 hour               :  Brainstorming with team
+1 hr                    :  Attended the soft skills session with HR team
+1.5 hr                    : Explored on Basics of Javascript  ( Script tags, Inlining,Syntax &amp; Popup Messages, DOM )                                                    </t>
   </si>
   <si>
     <t>Exploring angular</t>
@@ -7352,8 +7357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9136D698-C624-4D52-A3F8-D913404DF880}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7601,13 +7606,13 @@
         <v>158</v>
       </c>
       <c r="D15" s="47" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="E15" s="35" t="s">
         <v>41</v>
       </c>
       <c r="F15" s="45">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="G15" s="35">
         <v>0</v>
@@ -7619,10 +7624,10 @@
         <v>34</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D16" s="44" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E16" s="35"/>
       <c r="F16" s="35">

</xml_diff>

<commit_message>
Updated Time Sheet- Aravindhan
</commit_message>
<xml_diff>
--- a/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
+++ b/Process/Timesheet/TeamAlpha-Timesheet 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0AF5E792-69B1-4693-9623-7834FC5A300C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E26F3CD-1A73-4305-A274-D23647EDAC34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 3(06-04-2022)" sheetId="40" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Day10 ( 18-04-2022 )" sheetId="49" r:id="rId8"/>
     <sheet name="Day11 ( 19-04-2022 )" sheetId="51" r:id="rId9"/>
     <sheet name="Day12 ( 20-04-2022 )" sheetId="52" r:id="rId10"/>
+    <sheet name="Day13 ( 21-04-2022 )" sheetId="53" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="180">
   <si>
     <t>Column1</t>
   </si>
@@ -711,6 +712,15 @@
   <si>
     <t>1 hr : Brainstorming with Team mates
 1 hr : Softskill session                                                                         1.5  hr : Web API- Forms, history and storage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8:15AM-8:20AM -Checking Mails.
+8:45AM-9:00AM -Brainstorming with team.
+9:00AM-10:30AM -Worked on MVC Application(for Code Review)
+10:30AM-10:45AM-Break
+10:45AM-11:45AM- Prepared Non Functional requirements
+11:50AM-12:55PM-Brushed Up Concepts(for Code Review)
+</t>
   </si>
 </sst>
 </file>
@@ -1118,7 +1128,539 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="210">
+  <dxfs count="231">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="16"/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="16"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color rgb="FF000000"/>
+        </vertical>
+        <horizontal style="thin">
+          <color rgb="FF000000"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -6453,290 +6995,319 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B59126C7-EF4B-42B8-885B-D999B591F622}" name="Table2" displayName="Table2" ref="B9:H19" totalsRowShown="0" headerRowDxfId="209" dataDxfId="208" headerRowBorderDxfId="206" tableBorderDxfId="207" totalsRowBorderDxfId="205">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B59126C7-EF4B-42B8-885B-D999B591F622}" name="Table2" displayName="Table2" ref="B9:H19" totalsRowShown="0" headerRowDxfId="230" dataDxfId="229" headerRowBorderDxfId="227" tableBorderDxfId="228" totalsRowBorderDxfId="226">
   <autoFilter ref="B9:H19" xr:uid="{B59126C7-EF4B-42B8-885B-D999B591F622}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{52B5F38B-ABB3-47C0-BB3D-A29F2DE51CC7}" name="Resource Name" dataDxfId="204"/>
-    <tableColumn id="2" xr3:uid="{EE1FCD6C-E5A0-4CCC-B385-C1EFECE5FDAA}" name="In-progress" dataDxfId="203"/>
-    <tableColumn id="3" xr3:uid="{181E4433-047B-4DE4-8CA4-63F4C195E21B}" name="Done" dataDxfId="202"/>
-    <tableColumn id="4" xr3:uid="{3D6F0A13-3C98-4A4C-A37F-39C4F130B0FD}" name="Discarded / Hold" dataDxfId="201"/>
-    <tableColumn id="5" xr3:uid="{6C95647F-EC05-4637-9771-13884C172508}" name="Hours Spent - Project" dataDxfId="200"/>
-    <tableColumn id="6" xr3:uid="{61429939-C632-43F5-B197-7173C32B4F6F}" name="Hours Spent - Non Project" dataDxfId="199"/>
-    <tableColumn id="7" xr3:uid="{FA348B8C-B11C-46EA-A9B6-9E454AA967AA}" name="Comments" dataDxfId="198"/>
+    <tableColumn id="1" xr3:uid="{52B5F38B-ABB3-47C0-BB3D-A29F2DE51CC7}" name="Resource Name" dataDxfId="225"/>
+    <tableColumn id="2" xr3:uid="{EE1FCD6C-E5A0-4CCC-B385-C1EFECE5FDAA}" name="In-progress" dataDxfId="224"/>
+    <tableColumn id="3" xr3:uid="{181E4433-047B-4DE4-8CA4-63F4C195E21B}" name="Done" dataDxfId="223"/>
+    <tableColumn id="4" xr3:uid="{3D6F0A13-3C98-4A4C-A37F-39C4F130B0FD}" name="Discarded / Hold" dataDxfId="222"/>
+    <tableColumn id="5" xr3:uid="{6C95647F-EC05-4637-9771-13884C172508}" name="Hours Spent - Project" dataDxfId="221"/>
+    <tableColumn id="6" xr3:uid="{61429939-C632-43F5-B197-7173C32B4F6F}" name="Hours Spent - Non Project" dataDxfId="220"/>
+    <tableColumn id="7" xr3:uid="{FA348B8C-B11C-46EA-A9B6-9E454AA967AA}" name="Comments" dataDxfId="219"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D14697CD-D871-4BE9-9957-83E5498C6EE5}" name="Table3751113" displayName="Table3751113" ref="B2:E4" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112" headerRowBorderDxfId="110" tableBorderDxfId="111" totalsRowBorderDxfId="109">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D14697CD-D871-4BE9-9957-83E5498C6EE5}" name="Table3751113" displayName="Table3751113" ref="B2:E4" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133" headerRowBorderDxfId="131" tableBorderDxfId="132" totalsRowBorderDxfId="130">
   <autoFilter ref="B2:E4" xr:uid="{9D11D6AC-943D-4BD1-9800-DECD246F6E62}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{597AD08F-5CEE-486B-928A-4E0143DEB21C}" name="Column1" dataDxfId="108"/>
-    <tableColumn id="2" xr3:uid="{80BDA1F7-DDA4-494F-BB7E-61D9A6E30A98}" name="Column2" dataDxfId="107"/>
-    <tableColumn id="3" xr3:uid="{DF109DE4-28E3-4BB2-997F-34A3F319520E}" name="Column3" dataDxfId="106"/>
-    <tableColumn id="4" xr3:uid="{C98D2CDB-0DA6-4DBC-80D8-197F6DC8262F}" name="Column4" dataDxfId="105"/>
+    <tableColumn id="1" xr3:uid="{597AD08F-5CEE-486B-928A-4E0143DEB21C}" name="Column1" dataDxfId="129"/>
+    <tableColumn id="2" xr3:uid="{80BDA1F7-DDA4-494F-BB7E-61D9A6E30A98}" name="Column2" dataDxfId="128"/>
+    <tableColumn id="3" xr3:uid="{DF109DE4-28E3-4BB2-997F-34A3F319520E}" name="Column3" dataDxfId="127"/>
+    <tableColumn id="4" xr3:uid="{C98D2CDB-0DA6-4DBC-80D8-197F6DC8262F}" name="Column4" dataDxfId="126"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{A036296C-A09A-4538-8AEF-52AAB9228500}" name="Table2621014" displayName="Table2621014" ref="B7:H17" totalsRowShown="0" headerRowDxfId="104" dataDxfId="103" headerRowBorderDxfId="101" tableBorderDxfId="102" totalsRowBorderDxfId="100">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{A036296C-A09A-4538-8AEF-52AAB9228500}" name="Table2621014" displayName="Table2621014" ref="B7:H17" totalsRowShown="0" headerRowDxfId="125" dataDxfId="124" headerRowBorderDxfId="122" tableBorderDxfId="123" totalsRowBorderDxfId="121">
   <autoFilter ref="B7:H17" xr:uid="{A30D6EFF-9BA6-4C4E-A49E-6E01C92313FC}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{AF106EC2-9249-449D-84E6-7F225A50644A}" name="Resource Name" dataDxfId="99"/>
-    <tableColumn id="2" xr3:uid="{C5721F56-75DD-416B-8AF4-882B78C097A4}" name="In-progress" dataDxfId="98"/>
-    <tableColumn id="3" xr3:uid="{65371F98-F64C-4B19-8CA2-7EF266D44FBF}" name="Done" dataDxfId="97"/>
-    <tableColumn id="4" xr3:uid="{EDCBD646-6D4A-4D8E-A78F-13A92C55A829}" name="Discarded / Hold" dataDxfId="96"/>
-    <tableColumn id="5" xr3:uid="{5216518A-9337-493A-8FBE-8BB58C828250}" name="Hours Spent - Project" dataDxfId="95"/>
-    <tableColumn id="6" xr3:uid="{249FD4AA-FDB0-40B3-A254-56EFA2226474}" name="Hours Spent - Non Project" dataDxfId="94"/>
-    <tableColumn id="7" xr3:uid="{47669AF2-CA1E-4E4D-8758-1BE493ED8AF4}" name="Comments" dataDxfId="93"/>
+    <tableColumn id="1" xr3:uid="{AF106EC2-9249-449D-84E6-7F225A50644A}" name="Resource Name" dataDxfId="120"/>
+    <tableColumn id="2" xr3:uid="{C5721F56-75DD-416B-8AF4-882B78C097A4}" name="In-progress" dataDxfId="119"/>
+    <tableColumn id="3" xr3:uid="{65371F98-F64C-4B19-8CA2-7EF266D44FBF}" name="Done" dataDxfId="118"/>
+    <tableColumn id="4" xr3:uid="{EDCBD646-6D4A-4D8E-A78F-13A92C55A829}" name="Discarded / Hold" dataDxfId="117"/>
+    <tableColumn id="5" xr3:uid="{5216518A-9337-493A-8FBE-8BB58C828250}" name="Hours Spent - Project" dataDxfId="116"/>
+    <tableColumn id="6" xr3:uid="{249FD4AA-FDB0-40B3-A254-56EFA2226474}" name="Hours Spent - Non Project" dataDxfId="115"/>
+    <tableColumn id="7" xr3:uid="{47669AF2-CA1E-4E4D-8758-1BE493ED8AF4}" name="Comments" dataDxfId="114"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{7FA1E999-6830-41E9-8136-B3DD83876559}" name="Table3751115" displayName="Table3751115" ref="B2:E4" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91" headerRowBorderDxfId="89" tableBorderDxfId="90" totalsRowBorderDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{7FA1E999-6830-41E9-8136-B3DD83876559}" name="Table3751115" displayName="Table3751115" ref="B2:E4" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112" headerRowBorderDxfId="110" tableBorderDxfId="111" totalsRowBorderDxfId="109">
   <autoFilter ref="B2:E4" xr:uid="{9D11D6AC-943D-4BD1-9800-DECD246F6E62}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D67A75C6-50A5-4ED9-9562-707A5D717E14}" name="Column1" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{4CBEA24E-4C4B-4B23-85EB-4A8217A30752}" name="Column2" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{A13B37EF-4736-411C-BF75-CBDF316BAB90}" name="Column3" dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{504EFC7F-2F49-4D22-ACB4-DCD4F1C95FE1}" name="Column4" dataDxfId="84"/>
+    <tableColumn id="1" xr3:uid="{D67A75C6-50A5-4ED9-9562-707A5D717E14}" name="Column1" dataDxfId="108"/>
+    <tableColumn id="2" xr3:uid="{4CBEA24E-4C4B-4B23-85EB-4A8217A30752}" name="Column2" dataDxfId="107"/>
+    <tableColumn id="3" xr3:uid="{A13B37EF-4736-411C-BF75-CBDF316BAB90}" name="Column3" dataDxfId="106"/>
+    <tableColumn id="4" xr3:uid="{504EFC7F-2F49-4D22-ACB4-DCD4F1C95FE1}" name="Column4" dataDxfId="105"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A30D6EFF-9BA6-4C4E-A49E-6E01C92313FC}" name="Table26210" displayName="Table26210" ref="B7:H17" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82" headerRowBorderDxfId="80" tableBorderDxfId="81" totalsRowBorderDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{A30D6EFF-9BA6-4C4E-A49E-6E01C92313FC}" name="Table26210" displayName="Table26210" ref="B7:H17" totalsRowShown="0" headerRowDxfId="104" dataDxfId="103" headerRowBorderDxfId="101" tableBorderDxfId="102" totalsRowBorderDxfId="100">
   <autoFilter ref="B7:H17" xr:uid="{A30D6EFF-9BA6-4C4E-A49E-6E01C92313FC}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{CB514E32-07C5-40CB-B6EC-7CE1D7B57BF0}" name="Resource Name" dataDxfId="78"/>
-    <tableColumn id="2" xr3:uid="{C46C6E29-0824-4E17-8EAF-64A911996B4D}" name="In-progress" dataDxfId="77"/>
-    <tableColumn id="3" xr3:uid="{6B5DC81A-7A98-4BF7-864C-E5A79BB97505}" name="Done" dataDxfId="76"/>
-    <tableColumn id="4" xr3:uid="{0C243582-3F95-4A38-8545-76DB2898625E}" name="Discarded / Hold" dataDxfId="75"/>
-    <tableColumn id="5" xr3:uid="{FD3CD380-CAB0-422C-8CF7-6944378DDBE6}" name="Hours Spent - Project" dataDxfId="74"/>
-    <tableColumn id="6" xr3:uid="{145CB7BA-3D9C-44AC-9E51-716B58B77D2F}" name="Hours Spent - Non Project" dataDxfId="73"/>
-    <tableColumn id="7" xr3:uid="{507AE42A-A1CC-4934-90C2-3BFCE53238B3}" name="Comments" dataDxfId="72"/>
+    <tableColumn id="1" xr3:uid="{CB514E32-07C5-40CB-B6EC-7CE1D7B57BF0}" name="Resource Name" dataDxfId="99"/>
+    <tableColumn id="2" xr3:uid="{C46C6E29-0824-4E17-8EAF-64A911996B4D}" name="In-progress" dataDxfId="98"/>
+    <tableColumn id="3" xr3:uid="{6B5DC81A-7A98-4BF7-864C-E5A79BB97505}" name="Done" dataDxfId="97"/>
+    <tableColumn id="4" xr3:uid="{0C243582-3F95-4A38-8545-76DB2898625E}" name="Discarded / Hold" dataDxfId="96"/>
+    <tableColumn id="5" xr3:uid="{FD3CD380-CAB0-422C-8CF7-6944378DDBE6}" name="Hours Spent - Project" dataDxfId="95"/>
+    <tableColumn id="6" xr3:uid="{145CB7BA-3D9C-44AC-9E51-716B58B77D2F}" name="Hours Spent - Non Project" dataDxfId="94"/>
+    <tableColumn id="7" xr3:uid="{507AE42A-A1CC-4934-90C2-3BFCE53238B3}" name="Comments" dataDxfId="93"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9D11D6AC-943D-4BD1-9800-DECD246F6E62}" name="Table37511" displayName="Table37511" ref="B2:E4" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70" headerRowBorderDxfId="68" tableBorderDxfId="69" totalsRowBorderDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{9D11D6AC-943D-4BD1-9800-DECD246F6E62}" name="Table37511" displayName="Table37511" ref="B2:E4" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91" headerRowBorderDxfId="89" tableBorderDxfId="90" totalsRowBorderDxfId="88">
   <autoFilter ref="B2:E4" xr:uid="{9D11D6AC-943D-4BD1-9800-DECD246F6E62}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6B075576-4726-42C8-996A-A7B4B187D27F}" name="Column1" dataDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{2B0F43B9-480B-4C54-A4CC-3DFC00711929}" name="Column2" dataDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{4353F121-13EC-4653-AB7A-C0BBED71F612}" name="Column3" dataDxfId="64"/>
-    <tableColumn id="4" xr3:uid="{AD8279C5-6226-4ECF-A6C8-F9C70974EABE}" name="Column4" dataDxfId="63"/>
+    <tableColumn id="1" xr3:uid="{6B075576-4726-42C8-996A-A7B4B187D27F}" name="Column1" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{2B0F43B9-480B-4C54-A4CC-3DFC00711929}" name="Column2" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{4353F121-13EC-4653-AB7A-C0BBED71F612}" name="Column3" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{AD8279C5-6226-4ECF-A6C8-F9C70974EABE}" name="Column4" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{1356D4E1-15F0-41BF-B0C4-E4DC18B96A83}" name="Table2621016" displayName="Table2621016" ref="B7:H17" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61" headerRowBorderDxfId="59" tableBorderDxfId="60" totalsRowBorderDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{1356D4E1-15F0-41BF-B0C4-E4DC18B96A83}" name="Table2621016" displayName="Table2621016" ref="B7:H17" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82" headerRowBorderDxfId="80" tableBorderDxfId="81" totalsRowBorderDxfId="79">
   <autoFilter ref="B7:H17" xr:uid="{1356D4E1-15F0-41BF-B0C4-E4DC18B96A83}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{975CF6D7-F24C-4D9F-BA9F-439AF60EF114}" name="Resource Name" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{BC36331B-5C09-49F2-8E13-D5168DD28D0F}" name="In-progress" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{41B5A763-B80D-4E4B-976F-9969D2C0C14F}" name="Done" dataDxfId="55"/>
-    <tableColumn id="4" xr3:uid="{5D1F40BB-F239-4A1D-AEF6-82A5FC99D7CD}" name="Discarded / Hold" dataDxfId="54"/>
-    <tableColumn id="5" xr3:uid="{5C9549F2-9CF2-45B7-98E8-1D291B3630B2}" name="Hours Spent - Project" dataDxfId="53"/>
-    <tableColumn id="6" xr3:uid="{04DC6A6C-EEB6-4EF4-911D-C37E2C5B40FF}" name="Hours Spent - Non Project" dataDxfId="52"/>
-    <tableColumn id="7" xr3:uid="{C3902E87-CCB6-47C9-9BC1-FD0B37543238}" name="Comments" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{975CF6D7-F24C-4D9F-BA9F-439AF60EF114}" name="Resource Name" dataDxfId="78"/>
+    <tableColumn id="2" xr3:uid="{BC36331B-5C09-49F2-8E13-D5168DD28D0F}" name="In-progress" dataDxfId="77"/>
+    <tableColumn id="3" xr3:uid="{41B5A763-B80D-4E4B-976F-9969D2C0C14F}" name="Done" dataDxfId="76"/>
+    <tableColumn id="4" xr3:uid="{5D1F40BB-F239-4A1D-AEF6-82A5FC99D7CD}" name="Discarded / Hold" dataDxfId="75"/>
+    <tableColumn id="5" xr3:uid="{5C9549F2-9CF2-45B7-98E8-1D291B3630B2}" name="Hours Spent - Project" dataDxfId="74"/>
+    <tableColumn id="6" xr3:uid="{04DC6A6C-EEB6-4EF4-911D-C37E2C5B40FF}" name="Hours Spent - Non Project" dataDxfId="73"/>
+    <tableColumn id="7" xr3:uid="{C3902E87-CCB6-47C9-9BC1-FD0B37543238}" name="Comments" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E3497E54-1E59-44E7-9480-106E98FB838A}" name="Table3751117" displayName="Table3751117" ref="B2:E4" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49" headerRowBorderDxfId="47" tableBorderDxfId="48" totalsRowBorderDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E3497E54-1E59-44E7-9480-106E98FB838A}" name="Table3751117" displayName="Table3751117" ref="B2:E4" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70" headerRowBorderDxfId="68" tableBorderDxfId="69" totalsRowBorderDxfId="67">
   <autoFilter ref="B2:E4" xr:uid="{E3497E54-1E59-44E7-9480-106E98FB838A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{69E7B7B7-0FF3-43D1-AE4A-578CB3CCCFBD}" name="Column1" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{753FC1E8-1B96-4804-A794-92A8953D5EE2}" name="Column2" dataDxfId="44"/>
-    <tableColumn id="3" xr3:uid="{50B38A4B-BAF8-4640-8ECB-0900A6C915DB}" name="Column3" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{4432DCD0-98FF-4B59-BAB7-E3FE0A3EDFBC}" name="Column4" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{69E7B7B7-0FF3-43D1-AE4A-578CB3CCCFBD}" name="Column1" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{753FC1E8-1B96-4804-A794-92A8953D5EE2}" name="Column2" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{50B38A4B-BAF8-4640-8ECB-0900A6C915DB}" name="Column3" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{4432DCD0-98FF-4B59-BAB7-E3FE0A3EDFBC}" name="Column4" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{D3490739-1854-4802-BC7E-8F8A56938939}" name="Table262101618" displayName="Table262101618" ref="B7:H17" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" headerRowBorderDxfId="38" tableBorderDxfId="39" totalsRowBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{D3490739-1854-4802-BC7E-8F8A56938939}" name="Table262101618" displayName="Table262101618" ref="B7:H17" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61" headerRowBorderDxfId="59" tableBorderDxfId="60" totalsRowBorderDxfId="58">
   <autoFilter ref="B7:H17" xr:uid="{1356D4E1-15F0-41BF-B0C4-E4DC18B96A83}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F4CDC508-938F-4C7B-9D78-6C7897C95C75}" name="Resource Name" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{D24B5720-9179-4EA6-A1B2-11FFE3971AE0}" name="In-progress" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{38376D7D-1777-43ED-87F4-271C7CA93BC0}" name="Done" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{27CF804E-18A7-4ED9-9891-7FE4B93C6D6C}" name="Discarded / Hold" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{F23FF8B6-B301-4C5F-ACF3-3D16EEFFC3F0}" name="Hours Spent - Project" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{2D0142DB-38B6-4D6B-A60F-A9A19574C7ED}" name="Hours Spent - Non Project" dataDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{8BAC7AAB-A572-4256-AFEE-71DC94CC59B9}" name="Comments" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{F4CDC508-938F-4C7B-9D78-6C7897C95C75}" name="Resource Name" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{D24B5720-9179-4EA6-A1B2-11FFE3971AE0}" name="In-progress" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{38376D7D-1777-43ED-87F4-271C7CA93BC0}" name="Done" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{27CF804E-18A7-4ED9-9891-7FE4B93C6D6C}" name="Discarded / Hold" dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{F23FF8B6-B301-4C5F-ACF3-3D16EEFFC3F0}" name="Hours Spent - Project" dataDxfId="53"/>
+    <tableColumn id="6" xr3:uid="{2D0142DB-38B6-4D6B-A60F-A9A19574C7ED}" name="Hours Spent - Non Project" dataDxfId="52"/>
+    <tableColumn id="7" xr3:uid="{8BAC7AAB-A572-4256-AFEE-71DC94CC59B9}" name="Comments" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{65B9F601-45A2-418D-921A-3D56A32B6C21}" name="Table375111719" displayName="Table375111719" ref="B2:E4" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" headerRowBorderDxfId="26" tableBorderDxfId="27" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{65B9F601-45A2-418D-921A-3D56A32B6C21}" name="Table375111719" displayName="Table375111719" ref="B2:E4" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49" headerRowBorderDxfId="47" tableBorderDxfId="48" totalsRowBorderDxfId="46">
   <autoFilter ref="B2:E4" xr:uid="{E3497E54-1E59-44E7-9480-106E98FB838A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6E252E52-03A5-4570-990A-B3378296E039}" name="Column1" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{D5447885-EF1E-44FE-B1A4-EE1475056221}" name="Column2" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{2F816DC6-3307-4F6E-9962-EB8AB2F91C9F}" name="Column3" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{21AE6030-4E77-45A3-8CDA-342E87194417}" name="Column4" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{6E252E52-03A5-4570-990A-B3378296E039}" name="Column1" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{D5447885-EF1E-44FE-B1A4-EE1475056221}" name="Column2" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{2F816DC6-3307-4F6E-9962-EB8AB2F91C9F}" name="Column3" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{21AE6030-4E77-45A3-8CDA-342E87194417}" name="Column4" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{567599D8-F2AC-4863-A31E-867E4662A188}" name="Table26210161820" displayName="Table26210161820" ref="B7:H17" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{567599D8-F2AC-4863-A31E-867E4662A188}" name="Table26210161820" displayName="Table26210161820" ref="B7:H17" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" headerRowBorderDxfId="38" tableBorderDxfId="39" totalsRowBorderDxfId="37">
   <autoFilter ref="B7:H17" xr:uid="{1356D4E1-15F0-41BF-B0C4-E4DC18B96A83}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{6862ACD5-06E8-4C76-86B8-0FBF46C719AB}" name="Resource Name" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{2FEAF882-A5EF-4611-91BB-CAEDE2BD0142}" name="In-progress" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{FB3D921D-555F-47F7-9140-AB8143CB71BA}" name="Done" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{BD8867CA-8566-48C2-BDB8-839066AC235A}" name="Discarded / Hold" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{F71E5005-E794-436C-8ABB-93D21EB0BD11}" name="Hours Spent - Project" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{53117683-12E5-4475-8EE2-ECA8DBFEEF45}" name="Hours Spent - Non Project" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{A1C72867-09F6-497F-ACF5-1458D252B64F}" name="Comments" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{6862ACD5-06E8-4C76-86B8-0FBF46C719AB}" name="Resource Name" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{2FEAF882-A5EF-4611-91BB-CAEDE2BD0142}" name="In-progress" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{FB3D921D-555F-47F7-9140-AB8143CB71BA}" name="Done" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{BD8867CA-8566-48C2-BDB8-839066AC235A}" name="Discarded / Hold" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{F71E5005-E794-436C-8ABB-93D21EB0BD11}" name="Hours Spent - Project" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{53117683-12E5-4475-8EE2-ECA8DBFEEF45}" name="Hours Spent - Non Project" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{A1C72867-09F6-497F-ACF5-1458D252B64F}" name="Comments" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BF3C43CE-B630-4202-BD3A-6EE2D770899A}" name="Table3" displayName="Table3" ref="B4:E6" totalsRowShown="0" headerRowDxfId="197" dataDxfId="196" headerRowBorderDxfId="194" tableBorderDxfId="195" totalsRowBorderDxfId="193">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BF3C43CE-B630-4202-BD3A-6EE2D770899A}" name="Table3" displayName="Table3" ref="B4:E6" totalsRowShown="0" headerRowDxfId="218" dataDxfId="217" headerRowBorderDxfId="215" tableBorderDxfId="216" totalsRowBorderDxfId="214">
   <autoFilter ref="B4:E6" xr:uid="{BF3C43CE-B630-4202-BD3A-6EE2D770899A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{BE43EB49-4D5D-488E-9520-6CE4AC2E5C1B}" name="Column1" dataDxfId="192"/>
-    <tableColumn id="2" xr3:uid="{16DFD0E6-4C5E-443C-BF24-706A867EF798}" name="Column2" dataDxfId="191"/>
-    <tableColumn id="3" xr3:uid="{DC8A145E-C833-4BE6-BAE5-7E5E2AC2891C}" name="Column3" dataDxfId="190"/>
-    <tableColumn id="4" xr3:uid="{9454D612-74D7-428F-B9A0-7151862F7C2A}" name="Column4" dataDxfId="189"/>
+    <tableColumn id="1" xr3:uid="{BE43EB49-4D5D-488E-9520-6CE4AC2E5C1B}" name="Column1" dataDxfId="213"/>
+    <tableColumn id="2" xr3:uid="{16DFD0E6-4C5E-443C-BF24-706A867EF798}" name="Column2" dataDxfId="212"/>
+    <tableColumn id="3" xr3:uid="{DC8A145E-C833-4BE6-BAE5-7E5E2AC2891C}" name="Column3" dataDxfId="211"/>
+    <tableColumn id="4" xr3:uid="{9454D612-74D7-428F-B9A0-7151862F7C2A}" name="Column4" dataDxfId="210"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{3AB7E480-AA41-45EE-8BD2-799B66CF977F}" name="Table37511171921" displayName="Table37511171921" ref="B2:E4" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{3AB7E480-AA41-45EE-8BD2-799B66CF977F}" name="Table37511171921" displayName="Table37511171921" ref="B2:E4" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" headerRowBorderDxfId="26" tableBorderDxfId="27" totalsRowBorderDxfId="25">
   <autoFilter ref="B2:E4" xr:uid="{E3497E54-1E59-44E7-9480-106E98FB838A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5F5286EA-BF04-4F20-B734-0734EC625276}" name="Column1" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{2666153F-F4E8-45C3-9985-38E5471A82F0}" name="Column2" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{ED99E108-F673-4294-9E8D-A329582DF55B}" name="Column3" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{B0F02456-D0DE-4E93-9016-90FA89E16184}" name="Column4" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{5F5286EA-BF04-4F20-B734-0734EC625276}" name="Column1" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{2666153F-F4E8-45C3-9985-38E5471A82F0}" name="Column2" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{ED99E108-F673-4294-9E8D-A329582DF55B}" name="Column3" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{B0F02456-D0DE-4E93-9016-90FA89E16184}" name="Column4" dataDxfId="21"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{B3B21B26-64D8-4DAA-B271-41535AB5FBA0}" name="Table2621016182022" displayName="Table2621016182022" ref="B7:H17" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+  <autoFilter ref="B7:H17" xr:uid="{B3B21B26-64D8-4DAA-B271-41535AB5FBA0}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{F31F1358-1BCD-4E28-8DE6-55060AD83C78}" name="Resource Name" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{85795525-35CB-4867-B9E8-8424F3C504C7}" name="In-progress" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{14491860-1E0F-4FC2-B40C-7BFA09F08AD3}" name="Done" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{4121DE0A-E31D-4416-93C4-5D79C06CB436}" name="Discarded / Hold" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{42DAEAF5-4695-460C-A7C8-11CA5A06441F}" name="Hours Spent - Project" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{5A90E8D4-8EBC-413F-9D20-BC476DDDDA89}" name="Hours Spent - Non Project" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{CDA42C61-7D2B-4220-801B-18B140C01D85}" name="Comments" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{055B31DD-6299-4C3C-ACAC-24A5C69F0229}" name="Table3751117192123" displayName="Table3751117192123" ref="B2:E4" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+  <autoFilter ref="B2:E4" xr:uid="{055B31DD-6299-4C3C-ACAC-24A5C69F0229}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{A361ACD1-4939-41DE-8AA2-8A2C23550B5A}" name="Column1" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{ADE6E992-B56C-47A2-8484-0F95117DFA87}" name="Column2" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{5D6FC945-76E2-4A8F-A729-023221CFF273}" name="Column3" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{F5B29A6E-68F5-487F-AE11-943B1309598F}" name="Column4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{46BFD46F-1AD6-4EF9-9F4D-9841A6E71CD9}" name="Table26" displayName="Table26" ref="B8:H18" totalsRowShown="0" headerRowDxfId="188" dataDxfId="187" headerRowBorderDxfId="185" tableBorderDxfId="186" totalsRowBorderDxfId="184">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{46BFD46F-1AD6-4EF9-9F4D-9841A6E71CD9}" name="Table26" displayName="Table26" ref="B8:H18" totalsRowShown="0" headerRowDxfId="209" dataDxfId="208" headerRowBorderDxfId="206" tableBorderDxfId="207" totalsRowBorderDxfId="205">
   <autoFilter ref="B8:H18" xr:uid="{46BFD46F-1AD6-4EF9-9F4D-9841A6E71CD9}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{7428D5F6-9EE3-49C6-B1BE-E57BFF59C7B0}" name="Resource Name" dataDxfId="183"/>
-    <tableColumn id="2" xr3:uid="{8EF82413-9CDB-4809-98BD-913D08316031}" name="In-progress" dataDxfId="182"/>
-    <tableColumn id="3" xr3:uid="{B4E2F1CC-113D-4DBD-9D8F-AFFEF819725B}" name="Done" dataDxfId="181"/>
-    <tableColumn id="4" xr3:uid="{A8C1C667-3FF8-4B7C-AEC8-2DD543708DEA}" name="Discarded / Hold" dataDxfId="180"/>
-    <tableColumn id="5" xr3:uid="{DF5599B4-665D-4C1C-8DFF-80F68FB27D64}" name="Hours Spent - Project" dataDxfId="179"/>
-    <tableColumn id="6" xr3:uid="{EAD7742A-CE22-40A8-90BD-AB0C0555FA39}" name="Hours Spent - Non Project" dataDxfId="178"/>
-    <tableColumn id="7" xr3:uid="{52C2DA4C-9FFA-48AF-B36A-2837B9ED00F1}" name="Comments" dataDxfId="177"/>
+    <tableColumn id="1" xr3:uid="{7428D5F6-9EE3-49C6-B1BE-E57BFF59C7B0}" name="Resource Name" dataDxfId="204"/>
+    <tableColumn id="2" xr3:uid="{8EF82413-9CDB-4809-98BD-913D08316031}" name="In-progress" dataDxfId="203"/>
+    <tableColumn id="3" xr3:uid="{B4E2F1CC-113D-4DBD-9D8F-AFFEF819725B}" name="Done" dataDxfId="202"/>
+    <tableColumn id="4" xr3:uid="{A8C1C667-3FF8-4B7C-AEC8-2DD543708DEA}" name="Discarded / Hold" dataDxfId="201"/>
+    <tableColumn id="5" xr3:uid="{DF5599B4-665D-4C1C-8DFF-80F68FB27D64}" name="Hours Spent - Project" dataDxfId="200"/>
+    <tableColumn id="6" xr3:uid="{EAD7742A-CE22-40A8-90BD-AB0C0555FA39}" name="Hours Spent - Non Project" dataDxfId="199"/>
+    <tableColumn id="7" xr3:uid="{52C2DA4C-9FFA-48AF-B36A-2837B9ED00F1}" name="Comments" dataDxfId="198"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9997EBAF-6A71-418E-B851-C8B1915211B5}" name="Table37" displayName="Table37" ref="B3:E5" totalsRowShown="0" headerRowDxfId="176" dataDxfId="175" headerRowBorderDxfId="173" tableBorderDxfId="174" totalsRowBorderDxfId="172">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9997EBAF-6A71-418E-B851-C8B1915211B5}" name="Table37" displayName="Table37" ref="B3:E5" totalsRowShown="0" headerRowDxfId="197" dataDxfId="196" headerRowBorderDxfId="194" tableBorderDxfId="195" totalsRowBorderDxfId="193">
   <autoFilter ref="B3:E5" xr:uid="{9997EBAF-6A71-418E-B851-C8B1915211B5}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{7EDDA488-2881-4A15-9B9C-777D834D815F}" name="Column1" dataDxfId="171"/>
-    <tableColumn id="2" xr3:uid="{AFE02A3A-062D-4251-90A2-DA5D33B35508}" name="Column2" dataDxfId="170"/>
-    <tableColumn id="3" xr3:uid="{ED8EDBC8-15CC-4013-9D78-2DF925F82DCD}" name="Column3" dataDxfId="169"/>
-    <tableColumn id="4" xr3:uid="{62C95B61-46F3-42F7-A1B8-B69D37DD10DF}" name="Column4" dataDxfId="168"/>
+    <tableColumn id="1" xr3:uid="{7EDDA488-2881-4A15-9B9C-777D834D815F}" name="Column1" dataDxfId="192"/>
+    <tableColumn id="2" xr3:uid="{AFE02A3A-062D-4251-90A2-DA5D33B35508}" name="Column2" dataDxfId="191"/>
+    <tableColumn id="3" xr3:uid="{ED8EDBC8-15CC-4013-9D78-2DF925F82DCD}" name="Column3" dataDxfId="190"/>
+    <tableColumn id="4" xr3:uid="{62C95B61-46F3-42F7-A1B8-B69D37DD10DF}" name="Column4" dataDxfId="189"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{158FF28A-C282-456C-9B5E-C00624BAAA83}" name="Table2628" displayName="Table2628" ref="B7:H17" totalsRowShown="0" headerRowDxfId="167" dataDxfId="166" headerRowBorderDxfId="164" tableBorderDxfId="165" totalsRowBorderDxfId="163">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{158FF28A-C282-456C-9B5E-C00624BAAA83}" name="Table2628" displayName="Table2628" ref="B7:H17" totalsRowShown="0" headerRowDxfId="188" dataDxfId="187" headerRowBorderDxfId="185" tableBorderDxfId="186" totalsRowBorderDxfId="184">
   <autoFilter ref="B7:H17" xr:uid="{B1AE0DC9-D1F6-4E81-8D21-EBCF5F00B2B7}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{FA7FB678-9F12-498D-AC8C-EA3804FA6C35}" name="Resource Name" dataDxfId="162"/>
-    <tableColumn id="2" xr3:uid="{393B2B95-8815-4457-B760-B5E70FBBB0A5}" name="In-progress" dataDxfId="161"/>
-    <tableColumn id="3" xr3:uid="{400FD95F-D628-4B07-904B-1F5E11C584A9}" name="Done" dataDxfId="160"/>
-    <tableColumn id="4" xr3:uid="{DA6CAF01-4620-4AD9-8F22-C26934025345}" name="Discarded / Hold" dataDxfId="159"/>
-    <tableColumn id="5" xr3:uid="{D70C3DC4-AF79-4EA9-916E-2DDB8181B077}" name="Hours Spent - Project" dataDxfId="158"/>
-    <tableColumn id="6" xr3:uid="{BA92211F-9DF3-4897-86C0-5FE2D8FC9C28}" name="Hours Spent - Non Project" dataDxfId="157"/>
-    <tableColumn id="7" xr3:uid="{673B654E-8412-4BCE-9293-22370300F740}" name="Comments" dataDxfId="156"/>
+    <tableColumn id="1" xr3:uid="{FA7FB678-9F12-498D-AC8C-EA3804FA6C35}" name="Resource Name" dataDxfId="183"/>
+    <tableColumn id="2" xr3:uid="{393B2B95-8815-4457-B760-B5E70FBBB0A5}" name="In-progress" dataDxfId="182"/>
+    <tableColumn id="3" xr3:uid="{400FD95F-D628-4B07-904B-1F5E11C584A9}" name="Done" dataDxfId="181"/>
+    <tableColumn id="4" xr3:uid="{DA6CAF01-4620-4AD9-8F22-C26934025345}" name="Discarded / Hold" dataDxfId="180"/>
+    <tableColumn id="5" xr3:uid="{D70C3DC4-AF79-4EA9-916E-2DDB8181B077}" name="Hours Spent - Project" dataDxfId="179"/>
+    <tableColumn id="6" xr3:uid="{BA92211F-9DF3-4897-86C0-5FE2D8FC9C28}" name="Hours Spent - Non Project" dataDxfId="178"/>
+    <tableColumn id="7" xr3:uid="{673B654E-8412-4BCE-9293-22370300F740}" name="Comments" dataDxfId="177"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FE979438-BC3B-45D4-9D8F-CD3DAC132734}" name="Table3759" displayName="Table3759" ref="B2:E4" totalsRowShown="0" headerRowDxfId="155" dataDxfId="154" headerRowBorderDxfId="152" tableBorderDxfId="153" totalsRowBorderDxfId="151">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FE979438-BC3B-45D4-9D8F-CD3DAC132734}" name="Table3759" displayName="Table3759" ref="B2:E4" totalsRowShown="0" headerRowDxfId="176" dataDxfId="175" headerRowBorderDxfId="173" tableBorderDxfId="174" totalsRowBorderDxfId="172">
   <autoFilter ref="B2:E4" xr:uid="{ACFFF651-B126-4B94-92B4-F3166A18744A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D1B206E0-BC18-44C3-AC3A-E386EBC240DA}" name="Column1" dataDxfId="150"/>
-    <tableColumn id="2" xr3:uid="{93DD1EAA-9879-4D36-9385-C9A727E59F3F}" name="Column2" dataDxfId="149"/>
-    <tableColumn id="3" xr3:uid="{C1074E65-5D51-4E3A-B9B1-1AA797A29E27}" name="Column3" dataDxfId="148"/>
-    <tableColumn id="4" xr3:uid="{CB82D336-531C-4BB2-AC91-1CAC6E92E6B7}" name="Column4" dataDxfId="147"/>
+    <tableColumn id="1" xr3:uid="{D1B206E0-BC18-44C3-AC3A-E386EBC240DA}" name="Column1" dataDxfId="171"/>
+    <tableColumn id="2" xr3:uid="{93DD1EAA-9879-4D36-9385-C9A727E59F3F}" name="Column2" dataDxfId="170"/>
+    <tableColumn id="3" xr3:uid="{C1074E65-5D51-4E3A-B9B1-1AA797A29E27}" name="Column3" dataDxfId="169"/>
+    <tableColumn id="4" xr3:uid="{CB82D336-531C-4BB2-AC91-1CAC6E92E6B7}" name="Column4" dataDxfId="168"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B1AE0DC9-D1F6-4E81-8D21-EBCF5F00B2B7}" name="Table262" displayName="Table262" ref="B7:H17" totalsRowShown="0" headerRowDxfId="146" dataDxfId="145" headerRowBorderDxfId="143" tableBorderDxfId="144" totalsRowBorderDxfId="142">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B1AE0DC9-D1F6-4E81-8D21-EBCF5F00B2B7}" name="Table262" displayName="Table262" ref="B7:H17" totalsRowShown="0" headerRowDxfId="167" dataDxfId="166" headerRowBorderDxfId="164" tableBorderDxfId="165" totalsRowBorderDxfId="163">
   <autoFilter ref="B7:H17" xr:uid="{B1AE0DC9-D1F6-4E81-8D21-EBCF5F00B2B7}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{C24C31E7-7289-4E64-B819-B73CBC38AAAC}" name="Resource Name" dataDxfId="141"/>
-    <tableColumn id="2" xr3:uid="{C2273D93-238B-4CCC-98AC-F0B06523F5CE}" name="In-progress" dataDxfId="140"/>
-    <tableColumn id="3" xr3:uid="{6E415DE6-A560-4988-877C-F716F699E312}" name="Done" dataDxfId="139"/>
-    <tableColumn id="4" xr3:uid="{C38A0EE9-47CE-4E5B-9C99-2B87137F78B9}" name="Discarded / Hold" dataDxfId="138"/>
-    <tableColumn id="5" xr3:uid="{1CC43B5C-77FA-4CED-8807-3E180A90E311}" name="Hours Spent - Project" dataDxfId="137"/>
-    <tableColumn id="6" xr3:uid="{356B8038-BBED-4F7F-B7BF-005E853F97B5}" name="Hours Spent - Non Project" dataDxfId="136"/>
-    <tableColumn id="7" xr3:uid="{AEE4776A-A2C0-4A70-ABAC-CB24A44ABC91}" name="Comments" dataDxfId="135"/>
+    <tableColumn id="1" xr3:uid="{C24C31E7-7289-4E64-B819-B73CBC38AAAC}" name="Resource Name" dataDxfId="162"/>
+    <tableColumn id="2" xr3:uid="{C2273D93-238B-4CCC-98AC-F0B06523F5CE}" name="In-progress" dataDxfId="161"/>
+    <tableColumn id="3" xr3:uid="{6E415DE6-A560-4988-877C-F716F699E312}" name="Done" dataDxfId="160"/>
+    <tableColumn id="4" xr3:uid="{C38A0EE9-47CE-4E5B-9C99-2B87137F78B9}" name="Discarded / Hold" dataDxfId="159"/>
+    <tableColumn id="5" xr3:uid="{1CC43B5C-77FA-4CED-8807-3E180A90E311}" name="Hours Spent - Project" dataDxfId="158"/>
+    <tableColumn id="6" xr3:uid="{356B8038-BBED-4F7F-B7BF-005E853F97B5}" name="Hours Spent - Non Project" dataDxfId="157"/>
+    <tableColumn id="7" xr3:uid="{AEE4776A-A2C0-4A70-ABAC-CB24A44ABC91}" name="Comments" dataDxfId="156"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ACFFF651-B126-4B94-92B4-F3166A18744A}" name="Table375" displayName="Table375" ref="B2:E4" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133" headerRowBorderDxfId="131" tableBorderDxfId="132" totalsRowBorderDxfId="130">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ACFFF651-B126-4B94-92B4-F3166A18744A}" name="Table375" displayName="Table375" ref="B2:E4" totalsRowShown="0" headerRowDxfId="155" dataDxfId="154" headerRowBorderDxfId="152" tableBorderDxfId="153" totalsRowBorderDxfId="151">
   <autoFilter ref="B2:E4" xr:uid="{ACFFF651-B126-4B94-92B4-F3166A18744A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{83E614ED-6ABF-439F-A9B7-1518844696D4}" name="Column1" dataDxfId="129"/>
-    <tableColumn id="2" xr3:uid="{8840A839-8BBB-4DA6-9464-87D437F25D89}" name="Column2" dataDxfId="128"/>
-    <tableColumn id="3" xr3:uid="{ADAFE106-25BF-4F64-96D1-03AE2BD94818}" name="Column3" dataDxfId="127"/>
-    <tableColumn id="4" xr3:uid="{377D3DE4-F5C8-4A2C-99F9-A46F41134437}" name="Column4" dataDxfId="126"/>
+    <tableColumn id="1" xr3:uid="{83E614ED-6ABF-439F-A9B7-1518844696D4}" name="Column1" dataDxfId="150"/>
+    <tableColumn id="2" xr3:uid="{8840A839-8BBB-4DA6-9464-87D437F25D89}" name="Column2" dataDxfId="149"/>
+    <tableColumn id="3" xr3:uid="{ADAFE106-25BF-4F64-96D1-03AE2BD94818}" name="Column3" dataDxfId="148"/>
+    <tableColumn id="4" xr3:uid="{377D3DE4-F5C8-4A2C-99F9-A46F41134437}" name="Column4" dataDxfId="147"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{A3D18560-C428-4868-B5CA-EBD1BE9F0FAE}" name="Table2621012" displayName="Table2621012" ref="B7:H17" totalsRowShown="0" headerRowDxfId="125" dataDxfId="124" headerRowBorderDxfId="122" tableBorderDxfId="123" totalsRowBorderDxfId="121">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{A3D18560-C428-4868-B5CA-EBD1BE9F0FAE}" name="Table2621012" displayName="Table2621012" ref="B7:H17" totalsRowShown="0" headerRowDxfId="146" dataDxfId="145" headerRowBorderDxfId="143" tableBorderDxfId="144" totalsRowBorderDxfId="142">
   <autoFilter ref="B7:H17" xr:uid="{A30D6EFF-9BA6-4C4E-A49E-6E01C92313FC}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B99CA38C-6B70-44CB-94F1-34C0E18CAF38}" name="Resource Name" dataDxfId="120"/>
-    <tableColumn id="2" xr3:uid="{795625D3-DD18-4E77-8101-AB4369863885}" name="In-progress" dataDxfId="119"/>
-    <tableColumn id="3" xr3:uid="{F0C7DD64-C3AC-4A21-AA1F-AEAA2996C869}" name="Done" dataDxfId="118"/>
-    <tableColumn id="4" xr3:uid="{E1FC84EA-4ED4-4270-A149-E1E189A198C6}" name="Discarded / Hold" dataDxfId="117"/>
-    <tableColumn id="5" xr3:uid="{78CD14E8-1C2D-4CD1-A99E-E32FD07A85E3}" name="Hours Spent - Project" dataDxfId="116"/>
-    <tableColumn id="6" xr3:uid="{85ABF2B2-9FE1-4EFB-A748-B433E667EC67}" name="Hours Spent - Non Project" dataDxfId="115"/>
-    <tableColumn id="7" xr3:uid="{AA131BC6-5AD2-4A73-863A-093BE3A0E40F}" name="Comments" dataDxfId="114"/>
+    <tableColumn id="1" xr3:uid="{B99CA38C-6B70-44CB-94F1-34C0E18CAF38}" name="Resource Name" dataDxfId="141"/>
+    <tableColumn id="2" xr3:uid="{795625D3-DD18-4E77-8101-AB4369863885}" name="In-progress" dataDxfId="140"/>
+    <tableColumn id="3" xr3:uid="{F0C7DD64-C3AC-4A21-AA1F-AEAA2996C869}" name="Done" dataDxfId="139"/>
+    <tableColumn id="4" xr3:uid="{E1FC84EA-4ED4-4270-A149-E1E189A198C6}" name="Discarded / Hold" dataDxfId="138"/>
+    <tableColumn id="5" xr3:uid="{78CD14E8-1C2D-4CD1-A99E-E32FD07A85E3}" name="Hours Spent - Project" dataDxfId="137"/>
+    <tableColumn id="6" xr3:uid="{85ABF2B2-9FE1-4EFB-A748-B433E667EC67}" name="Hours Spent - Non Project" dataDxfId="136"/>
+    <tableColumn id="7" xr3:uid="{AA131BC6-5AD2-4A73-863A-093BE3A0E40F}" name="Comments" dataDxfId="135"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7388,8 +7959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9136D698-C624-4D52-A3F8-D913404DF880}">
   <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7506,6 +8077,323 @@
       </c>
       <c r="G8" s="35">
         <v>2</v>
+      </c>
+      <c r="H8" s="23"/>
+    </row>
+    <row r="9" spans="1:8" ht="185.25" customHeight="1">
+      <c r="B9" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="35">
+        <v>2</v>
+      </c>
+      <c r="G9" s="35">
+        <v>1.2</v>
+      </c>
+      <c r="H9" s="24"/>
+    </row>
+    <row r="10" spans="1:8" ht="147" customHeight="1">
+      <c r="B10" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="35">
+        <v>2</v>
+      </c>
+      <c r="G10" s="35">
+        <v>1.2</v>
+      </c>
+      <c r="H10" s="24"/>
+    </row>
+    <row r="11" spans="1:8" ht="229.5" customHeight="1">
+      <c r="B11" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="35">
+        <v>4</v>
+      </c>
+      <c r="G11" s="35">
+        <v>0</v>
+      </c>
+      <c r="H11" s="25"/>
+    </row>
+    <row r="12" spans="1:8" ht="186.75" customHeight="1">
+      <c r="B12" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="25"/>
+    </row>
+    <row r="13" spans="1:8" ht="192" customHeight="1">
+      <c r="B13" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>171</v>
+      </c>
+      <c r="D13" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="35">
+        <v>2</v>
+      </c>
+      <c r="G13" s="35">
+        <v>1.2</v>
+      </c>
+      <c r="H13" s="25"/>
+    </row>
+    <row r="14" spans="1:8" ht="197.25" customHeight="1">
+      <c r="B14" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="35">
+        <v>3</v>
+      </c>
+      <c r="G14" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="25"/>
+    </row>
+    <row r="15" spans="1:8" ht="196.5" customHeight="1">
+      <c r="B15" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="D15" s="47" t="s">
+        <v>174</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="G15" s="35">
+        <v>1.2</v>
+      </c>
+      <c r="H15" s="26"/>
+    </row>
+    <row r="16" spans="1:8" ht="197.25" customHeight="1">
+      <c r="B16" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35">
+        <v>2</v>
+      </c>
+      <c r="G16" s="35">
+        <v>1.2</v>
+      </c>
+      <c r="H16" s="27"/>
+    </row>
+    <row r="17" spans="2:8" ht="273.75" customHeight="1">
+      <c r="B17" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>177</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="42">
+        <v>2.5</v>
+      </c>
+      <c r="G17" s="42">
+        <v>1</v>
+      </c>
+      <c r="H17" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164F129C-4B66-4886-90DA-03408C042996}">
+  <dimension ref="A2:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" customWidth="1"/>
+    <col min="4" max="4" width="68.7109375" customWidth="1"/>
+    <col min="5" max="5" width="62.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" ht="21">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" ht="21">
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" ht="21">
+      <c r="B4" s="6"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" ht="21">
+      <c r="B5" s="4"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" ht="20.25">
+      <c r="B6" s="11"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="41.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="219.75" customHeight="1">
+      <c r="B8" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="35">
+        <v>1</v>
+      </c>
+      <c r="G8" s="35">
+        <v>2.2000000000000002</v>
       </c>
       <c r="H8" s="23"/>
     </row>

</xml_diff>